<commit_message>
Update Sanity Check for User Research
Removed GLLinItems.zip and uploaded it to jam.
Updated Sanity check to point to zip on jam.
</commit_message>
<xml_diff>
--- a/test/testcase/NORMAN Sanity Check.xlsx
+++ b/test/testcase/NORMAN Sanity Check.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="14320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25365" windowHeight="14325" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisite" sheetId="6" r:id="rId1"/>
@@ -485,9 +485,6 @@
     <t>File explorer should open</t>
   </si>
   <si>
-    <t>Select GLLinItems.zip from \Norman\test\testcase\</t>
-  </si>
-  <si>
     <t>Processing dialog should appear until upload is complete</t>
   </si>
   <si>
@@ -753,6 +750,9 @@
   </si>
   <si>
     <t>Add an Angular control (Not applicable for now)</t>
+  </si>
+  <si>
+    <t>Select GLLinItems.zip (download from Jam here: https://jam4.sapjam.com/groups/60qDosrRAVDTLeeirVt451/content?folder_id=HuhlwTf9pwlyZHuNTugZ6J )</t>
   </si>
 </sst>
 </file>
@@ -4063,22 +4063,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="76.6640625" customWidth="1"/>
+    <col min="2" max="2" width="76.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30">
+    <row r="1" spans="1:2" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="24" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" ht="15" thickBot="1">
+    <row r="4" spans="1:2" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="22" customFormat="1" ht="21" thickBot="1">
+    <row r="5" spans="1:2" s="22" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="22">
         <v>1</v>
       </c>
@@ -4094,7 +4094,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="22" customFormat="1" ht="21" thickBot="1">
+    <row r="6" spans="1:2" s="22" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="22">
         <v>2</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="22" customFormat="1" ht="21" thickBot="1">
+    <row r="7" spans="1:2" s="22" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="22">
         <v>3</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <v>3.1</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>3.2</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
         <v>3.3</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>3.4</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="39">
         <v>3.5</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
         <v>116</v>
       </c>
@@ -4158,13 +4158,13 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
       <c r="B14" s="43" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
     </row>
   </sheetData>
@@ -4182,30 +4182,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.83203125" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="94.5" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="94.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B1" s="24" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28">
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -4220,7 +4220,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:7" ht="21" thickBot="1">
+    <row r="6" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -4233,7 +4233,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="20">
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -4246,7 +4246,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
         <v>1</v>
@@ -4257,7 +4257,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7" t="s">
         <v>0</v>
@@ -4268,7 +4268,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="11" t="s">
         <v>9</v>
@@ -4279,7 +4279,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" ht="141" customHeight="1" thickBot="1">
+    <row r="11" spans="1:7" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13" t="s">
         <v>10</v>
@@ -4290,7 +4290,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="20">
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -4303,7 +4303,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="9"/>
       <c r="C13" s="11" t="s">
@@ -4314,7 +4314,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="16"/>
       <c r="C14" s="11" t="s">
@@ -4325,7 +4325,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="17"/>
       <c r="C15" s="11" t="s">
@@ -4336,18 +4336,18 @@
       <c r="F15" s="11"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -4356,7 +4356,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -4365,7 +4365,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="180" customHeight="1" thickBot="1">
+    <row r="19" spans="1:7" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -4374,7 +4374,7 @@
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="20">
+    <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>4</v>
       </c>
@@ -4387,7 +4387,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="16" t="s">
         <v>15</v>
@@ -4400,29 +4400,29 @@
       <c r="F21" s="11"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="16"/>
       <c r="C22" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="16"/>
       <c r="C23" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -4431,7 +4431,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -4440,7 +4440,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -4449,7 +4449,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -4458,7 +4458,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -4467,7 +4467,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -4476,7 +4476,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -4485,7 +4485,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -4494,7 +4494,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="123" customHeight="1" thickBot="1">
+    <row r="32" spans="1:7" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="19"/>
       <c r="C32" s="13"/>
@@ -4503,7 +4503,7 @@
       <c r="F32" s="13"/>
       <c r="G32" s="14"/>
     </row>
-    <row r="33" spans="1:7" ht="20">
+    <row r="33" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>5</v>
       </c>
@@ -4516,7 +4516,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="16" t="s">
         <v>19</v>
@@ -4529,7 +4529,7 @@
       <c r="F34" s="11"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="16"/>
       <c r="C35" s="11" t="s">
@@ -4540,29 +4540,29 @@
       <c r="F35" s="11"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="16"/>
       <c r="C36" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="11"/>
       <c r="C37" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -4571,7 +4571,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -4580,7 +4580,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -4589,7 +4589,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -4598,7 +4598,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -4607,7 +4607,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -4616,7 +4616,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -4625,7 +4625,7 @@
       <c r="F44" s="11"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="124" customHeight="1" thickBot="1">
+    <row r="45" spans="1:7" ht="123.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="19"/>
       <c r="C45" s="13"/>
@@ -4634,12 +4634,12 @@
       <c r="F45" s="13"/>
       <c r="G45" s="14"/>
     </row>
-    <row r="46" spans="1:7" ht="20">
+    <row r="46" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>6</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="11"/>
@@ -4647,7 +4647,7 @@
       <c r="F46" s="11"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="16" t="s">
         <v>22</v>
@@ -4660,7 +4660,7 @@
       <c r="F47" s="11"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
@@ -4668,7 +4668,7 @@
       <c r="F48" s="11"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="16"/>
       <c r="C49" s="11"/>
@@ -4677,7 +4677,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -4686,7 +4686,7 @@
       <c r="F50" s="11"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -4695,7 +4695,7 @@
       <c r="F51" s="11"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -4704,7 +4704,7 @@
       <c r="F52" s="11"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -4713,7 +4713,7 @@
       <c r="F53" s="11"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -4722,7 +4722,7 @@
       <c r="F54" s="11"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
@@ -4731,7 +4731,7 @@
       <c r="F55" s="11"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -4740,7 +4740,7 @@
       <c r="F56" s="11"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="16" t="s">
         <v>23</v>
@@ -4753,7 +4753,7 @@
       <c r="F57" s="11"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="124" customHeight="1" thickBot="1">
+    <row r="58" spans="1:7" ht="123.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
       <c r="B58" s="19"/>
       <c r="C58" s="13"/>
@@ -4762,12 +4762,12 @@
       <c r="F58" s="13"/>
       <c r="G58" s="14"/>
     </row>
-    <row r="59" spans="1:7" ht="20">
+    <row r="59" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="4">
         <v>7</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C59" s="21"/>
       <c r="D59" s="11"/>
@@ -4775,7 +4775,7 @@
       <c r="F59" s="11"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="16" t="s">
         <v>25</v>
@@ -4788,7 +4788,7 @@
       <c r="F60" s="11"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="16"/>
       <c r="C61" s="11"/>
@@ -4797,7 +4797,7 @@
       <c r="F61" s="11"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="16"/>
       <c r="C62" s="11"/>
@@ -4806,7 +4806,7 @@
       <c r="F62" s="11"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -4815,7 +4815,7 @@
       <c r="F63" s="11"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -4824,7 +4824,7 @@
       <c r="F64" s="11"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
@@ -4833,7 +4833,7 @@
       <c r="F65" s="11"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="11"/>
       <c r="C66" s="11"/>
@@ -4842,7 +4842,7 @@
       <c r="F66" s="11"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
@@ -4851,7 +4851,7 @@
       <c r="F67" s="11"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="11"/>
       <c r="C68" s="11"/>
@@ -4860,7 +4860,7 @@
       <c r="F68" s="11"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="11"/>
       <c r="C69" s="11"/>
@@ -4869,7 +4869,7 @@
       <c r="F69" s="11"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="11"/>
       <c r="C70" s="11"/>
@@ -4878,7 +4878,7 @@
       <c r="F70" s="11"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15" customHeight="1" thickBot="1">
+    <row r="71" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="19"/>
       <c r="C71" s="13"/>
@@ -4887,7 +4887,7 @@
       <c r="F71" s="13"/>
       <c r="G71" s="14"/>
     </row>
-    <row r="72" spans="1:7" ht="20">
+    <row r="72" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A72" s="4">
         <v>8</v>
       </c>
@@ -4900,7 +4900,7 @@
       <c r="F72" s="11"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="16" t="s">
         <v>27</v>
@@ -4913,7 +4913,7 @@
       <c r="F73" s="11"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="16"/>
       <c r="C74" s="11" t="s">
@@ -4924,7 +4924,7 @@
       <c r="F74" s="11"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="16"/>
       <c r="D75" s="11"/>
@@ -4932,7 +4932,7 @@
       <c r="F75" s="11"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="11"/>
       <c r="C76" s="11"/>
@@ -4941,7 +4941,7 @@
       <c r="F76" s="11"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -4950,7 +4950,7 @@
       <c r="F77" s="11"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="11"/>
       <c r="C78" s="11"/>
@@ -4959,7 +4959,7 @@
       <c r="F78" s="11"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="11"/>
       <c r="C79" s="11"/>
@@ -4968,7 +4968,7 @@
       <c r="F79" s="11"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="11"/>
       <c r="C80" s="11"/>
@@ -4977,7 +4977,7 @@
       <c r="F80" s="11"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="11"/>
       <c r="C81" s="11"/>
@@ -4986,7 +4986,7 @@
       <c r="F81" s="11"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="11"/>
       <c r="C82" s="11"/>
@@ -4995,7 +4995,7 @@
       <c r="F82" s="11"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="11"/>
       <c r="C83" s="11"/>
@@ -5004,7 +5004,7 @@
       <c r="F83" s="11"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="56" customHeight="1" thickBot="1">
+    <row r="84" spans="1:7" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12"/>
       <c r="B84" s="19"/>
       <c r="C84" s="13"/>
@@ -5013,7 +5013,7 @@
       <c r="F84" s="13"/>
       <c r="G84" s="14"/>
     </row>
-    <row r="85" spans="1:7" ht="20">
+    <row r="85" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A85" s="4">
         <v>9</v>
       </c>
@@ -5026,7 +5026,7 @@
       <c r="F85" s="11"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="16" t="s">
         <v>31</v>
@@ -5039,7 +5039,7 @@
       <c r="F86" s="11"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="16"/>
       <c r="C87" t="s">
@@ -5050,7 +5050,7 @@
       <c r="F87" s="11"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="16"/>
       <c r="D88" s="11"/>
@@ -5058,7 +5058,7 @@
       <c r="F88" s="11"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="11"/>
       <c r="C89" s="11"/>
@@ -5067,7 +5067,7 @@
       <c r="F89" s="11"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="11"/>
       <c r="C90" s="11"/>
@@ -5076,7 +5076,7 @@
       <c r="F90" s="11"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="11"/>
       <c r="C91" s="11"/>
@@ -5085,7 +5085,7 @@
       <c r="F91" s="11"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
@@ -5094,7 +5094,7 @@
       <c r="F92" s="11"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
@@ -5103,7 +5103,7 @@
       <c r="F93" s="11"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="11"/>
       <c r="C94" s="11"/>
@@ -5112,7 +5112,7 @@
       <c r="F94" s="11"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="11"/>
       <c r="C95" s="11"/>
@@ -5121,7 +5121,7 @@
       <c r="F95" s="11"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="11"/>
       <c r="C96" s="11"/>
@@ -5130,7 +5130,7 @@
       <c r="F96" s="11"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="56" customHeight="1" thickBot="1">
+    <row r="97" spans="1:7" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12"/>
       <c r="B97" s="19"/>
       <c r="C97" s="13"/>
@@ -5139,7 +5139,7 @@
       <c r="F97" s="13"/>
       <c r="G97" s="14"/>
     </row>
-    <row r="98" spans="1:7" ht="20">
+    <row r="98" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A98" s="4">
         <v>10</v>
       </c>
@@ -5152,7 +5152,7 @@
       <c r="F98" s="11"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="B99" s="16" t="s">
         <v>11</v>
@@ -5165,14 +5165,14 @@
       <c r="F99" s="11"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="16"/>
       <c r="D101" s="11"/>
@@ -5180,7 +5180,7 @@
       <c r="F101" s="11"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
       <c r="B102" s="11"/>
       <c r="C102" s="11"/>
@@ -5189,7 +5189,7 @@
       <c r="F102" s="11"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="11"/>
       <c r="C103" s="11"/>
@@ -5198,7 +5198,7 @@
       <c r="F103" s="11"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="11"/>
       <c r="C104" s="11"/>
@@ -5207,7 +5207,7 @@
       <c r="F104" s="11"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="11"/>
       <c r="C105" s="11"/>
@@ -5216,7 +5216,7 @@
       <c r="F105" s="11"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
       <c r="B106" s="11"/>
       <c r="C106" s="11"/>
@@ -5225,7 +5225,7 @@
       <c r="F106" s="11"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="11"/>
       <c r="C107" s="11"/>
@@ -5234,7 +5234,7 @@
       <c r="F107" s="11"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
@@ -5243,7 +5243,7 @@
       <c r="F108" s="11"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="16" t="s">
         <v>7</v>
@@ -5256,7 +5256,7 @@
       <c r="F109" s="11"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="170" customHeight="1" thickBot="1">
+    <row r="110" spans="1:7" ht="170.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>
       <c r="B110" s="19"/>
       <c r="C110" s="13"/>
@@ -5265,7 +5265,7 @@
       <c r="F110" s="13"/>
       <c r="G110" s="14"/>
     </row>
-    <row r="111" spans="1:7" ht="20">
+    <row r="111" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A111" s="4">
         <v>11</v>
       </c>
@@ -5278,7 +5278,7 @@
       <c r="F111" s="11"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
       <c r="B112" s="7" t="s">
         <v>41</v>
@@ -5288,7 +5288,7 @@
       <c r="F112" s="11"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
       <c r="B113" s="16" t="s">
         <v>39</v>
@@ -5301,14 +5301,14 @@
       <c r="F113" s="11"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
       <c r="F114" s="11"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
       <c r="B115" s="11"/>
       <c r="C115" s="11"/>
@@ -5317,7 +5317,7 @@
       <c r="F115" s="11"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="6"/>
       <c r="B116" s="11"/>
       <c r="C116" s="11"/>
@@ -5326,7 +5326,7 @@
       <c r="F116" s="11"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
       <c r="B117" s="11"/>
       <c r="C117" s="11"/>
@@ -5335,7 +5335,7 @@
       <c r="F117" s="11"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="6"/>
       <c r="B118" s="11"/>
       <c r="C118" s="11"/>
@@ -5344,7 +5344,7 @@
       <c r="F118" s="11"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
       <c r="B119" s="11"/>
       <c r="C119" s="11"/>
@@ -5353,7 +5353,7 @@
       <c r="F119" s="11"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="6"/>
       <c r="B120" s="11"/>
       <c r="C120" s="11"/>
@@ -5362,7 +5362,7 @@
       <c r="F120" s="11"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
       <c r="B121" s="11"/>
       <c r="C121" s="11"/>
@@ -5371,7 +5371,7 @@
       <c r="F121" s="11"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="6"/>
       <c r="B122" s="16" t="s">
         <v>43</v>
@@ -5382,7 +5382,7 @@
       <c r="F122" s="11"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
       <c r="B123" s="25" t="s">
         <v>44</v>
@@ -5393,7 +5393,7 @@
       <c r="F123" s="11"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="20" customHeight="1">
+    <row r="124" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="6"/>
       <c r="B124" s="26" t="s">
         <v>45</v>
@@ -5406,7 +5406,7 @@
       <c r="F124" s="11"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="17" customHeight="1">
+    <row r="125" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
       <c r="B125" s="26"/>
       <c r="C125" s="11" t="s">
@@ -5417,7 +5417,7 @@
       <c r="F125" s="11"/>
       <c r="G125" s="8"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="6"/>
       <c r="B126" s="26"/>
       <c r="C126" s="11" t="s">
@@ -5428,7 +5428,7 @@
       <c r="F126" s="11"/>
       <c r="G126" s="8"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="6"/>
       <c r="B127" s="26"/>
       <c r="C127" s="11"/>
@@ -5437,7 +5437,7 @@
       <c r="F127" s="11"/>
       <c r="G127" s="8"/>
     </row>
-    <row r="128" spans="1:7" ht="170" customHeight="1" thickBot="1">
+    <row r="128" spans="1:7" ht="170.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="12"/>
       <c r="B128" s="19"/>
       <c r="C128" s="13"/>
@@ -5446,7 +5446,7 @@
       <c r="F128" s="13"/>
       <c r="G128" s="14"/>
     </row>
-    <row r="129" spans="1:7" ht="20">
+    <row r="129" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A129" s="4">
         <v>12</v>
       </c>
@@ -5459,7 +5459,7 @@
       <c r="F129" s="11"/>
       <c r="G129" s="8"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="6"/>
       <c r="B130" s="7" t="s">
         <v>50</v>
@@ -5469,7 +5469,7 @@
       <c r="F130" s="11"/>
       <c r="G130" s="8"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="6"/>
       <c r="B131" s="16"/>
       <c r="D131" s="11"/>
@@ -5477,14 +5477,14 @@
       <c r="F131" s="11"/>
       <c r="G131" s="8"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="6"/>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
       <c r="G132" s="8"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="6"/>
       <c r="B133" s="11"/>
       <c r="C133" s="11"/>
@@ -5493,7 +5493,7 @@
       <c r="F133" s="11"/>
       <c r="G133" s="8"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="6"/>
       <c r="B134" s="11"/>
       <c r="C134" s="11"/>
@@ -5502,7 +5502,7 @@
       <c r="F134" s="11"/>
       <c r="G134" s="8"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="6"/>
       <c r="B135" s="11"/>
       <c r="C135" s="11"/>
@@ -5511,7 +5511,7 @@
       <c r="F135" s="11"/>
       <c r="G135" s="8"/>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="6"/>
       <c r="B136" s="11"/>
       <c r="C136" s="11"/>
@@ -5520,7 +5520,7 @@
       <c r="F136" s="11"/>
       <c r="G136" s="8"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="6"/>
       <c r="B137" s="11"/>
       <c r="C137" s="11"/>
@@ -5529,7 +5529,7 @@
       <c r="F137" s="11"/>
       <c r="G137" s="8"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="6"/>
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
@@ -5538,7 +5538,7 @@
       <c r="F138" s="11"/>
       <c r="G138" s="8"/>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="6"/>
       <c r="B139" s="11"/>
       <c r="C139" s="11"/>
@@ -5547,7 +5547,7 @@
       <c r="F139" s="11"/>
       <c r="G139" s="8"/>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="6"/>
       <c r="B140" s="16"/>
       <c r="C140" s="11"/>
@@ -5556,7 +5556,7 @@
       <c r="F140" s="11"/>
       <c r="G140" s="8"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="6"/>
       <c r="B141" s="25"/>
       <c r="C141" s="11"/>
@@ -5565,7 +5565,7 @@
       <c r="F141" s="11"/>
       <c r="G141" s="8"/>
     </row>
-    <row r="142" spans="1:7" ht="20" customHeight="1">
+    <row r="142" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
       <c r="B142" s="26"/>
       <c r="D142" s="11"/>
@@ -5573,7 +5573,7 @@
       <c r="F142" s="11"/>
       <c r="G142" s="8"/>
     </row>
-    <row r="143" spans="1:7" ht="17" customHeight="1">
+    <row r="143" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
       <c r="B143" s="26"/>
       <c r="C143" s="11"/>
@@ -5582,7 +5582,7 @@
       <c r="F143" s="11"/>
       <c r="G143" s="8"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="6"/>
       <c r="B144" s="26"/>
       <c r="C144" s="11"/>
@@ -5591,7 +5591,7 @@
       <c r="F144" s="11"/>
       <c r="G144" s="8"/>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="6"/>
       <c r="B145" s="26"/>
       <c r="C145" s="11"/>
@@ -5600,7 +5600,7 @@
       <c r="F145" s="11"/>
       <c r="G145" s="8"/>
     </row>
-    <row r="146" spans="1:7" ht="22" customHeight="1" thickBot="1">
+    <row r="146" spans="1:7" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="12"/>
       <c r="B146" s="19"/>
       <c r="C146" s="13"/>
@@ -5609,7 +5609,7 @@
       <c r="F146" s="13"/>
       <c r="G146" s="14"/>
     </row>
-    <row r="147" spans="1:7" ht="20">
+    <row r="147" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A147" s="4">
         <v>11</v>
       </c>
@@ -5622,7 +5622,7 @@
       <c r="F147" s="11"/>
       <c r="G147" s="8"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="6"/>
       <c r="B148" s="7" t="s">
         <v>40</v>
@@ -5635,7 +5635,7 @@
       <c r="F148" s="11"/>
       <c r="G148" s="8"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="6"/>
       <c r="B149" s="16"/>
       <c r="D149" s="11"/>
@@ -5643,14 +5643,14 @@
       <c r="F149" s="11"/>
       <c r="G149" s="8"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="6"/>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
       <c r="F150" s="11"/>
       <c r="G150" s="8"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="6"/>
       <c r="B151" s="11"/>
       <c r="C151" s="11"/>
@@ -5659,7 +5659,7 @@
       <c r="F151" s="11"/>
       <c r="G151" s="8"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="6"/>
       <c r="B152" s="11"/>
       <c r="C152" s="11"/>
@@ -5668,7 +5668,7 @@
       <c r="F152" s="11"/>
       <c r="G152" s="8"/>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="6"/>
       <c r="B153" s="11"/>
       <c r="C153" s="11"/>
@@ -5677,7 +5677,7 @@
       <c r="F153" s="11"/>
       <c r="G153" s="8"/>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="6"/>
       <c r="B154" s="11"/>
       <c r="C154" s="11"/>
@@ -5686,7 +5686,7 @@
       <c r="F154" s="11"/>
       <c r="G154" s="8"/>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="6"/>
       <c r="B155" s="11"/>
       <c r="C155" s="11"/>
@@ -5695,7 +5695,7 @@
       <c r="F155" s="11"/>
       <c r="G155" s="8"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="6"/>
       <c r="B156" s="11"/>
       <c r="C156" s="11"/>
@@ -5704,7 +5704,7 @@
       <c r="F156" s="11"/>
       <c r="G156" s="8"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="6"/>
       <c r="B157" s="11"/>
       <c r="C157" s="11"/>
@@ -5713,7 +5713,7 @@
       <c r="F157" s="11"/>
       <c r="G157" s="8"/>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="6"/>
       <c r="B158" s="16"/>
       <c r="C158" s="11"/>
@@ -5722,7 +5722,7 @@
       <c r="F158" s="11"/>
       <c r="G158" s="8"/>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="6"/>
       <c r="B159" s="25"/>
       <c r="C159" s="11"/>
@@ -5731,7 +5731,7 @@
       <c r="F159" s="11"/>
       <c r="G159" s="8"/>
     </row>
-    <row r="160" spans="1:7" ht="20" customHeight="1">
+    <row r="160" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="6"/>
       <c r="B160" s="26"/>
       <c r="D160" s="11"/>
@@ -5739,7 +5739,7 @@
       <c r="F160" s="11"/>
       <c r="G160" s="8"/>
     </row>
-    <row r="161" spans="1:7" ht="17" customHeight="1">
+    <row r="161" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="6"/>
       <c r="B161" s="26"/>
       <c r="C161" s="11"/>
@@ -5748,7 +5748,7 @@
       <c r="F161" s="11"/>
       <c r="G161" s="8"/>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="6"/>
       <c r="B162" s="26" t="s">
         <v>53</v>
@@ -5761,7 +5761,7 @@
       <c r="F162" s="11"/>
       <c r="G162" s="8"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="6"/>
       <c r="B163" s="26"/>
       <c r="C163" s="11"/>
@@ -5770,7 +5770,7 @@
       <c r="F163" s="11"/>
       <c r="G163" s="8"/>
     </row>
-    <row r="164" spans="1:7" ht="206" customHeight="1" thickBot="1">
+    <row r="164" spans="1:7" ht="206.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="12"/>
       <c r="B164" s="19"/>
       <c r="C164" s="13"/>
@@ -5779,7 +5779,7 @@
       <c r="F164" s="13"/>
       <c r="G164" s="14"/>
     </row>
-    <row r="165" spans="1:7" ht="20">
+    <row r="165" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A165" s="4">
         <v>12</v>
       </c>
@@ -5792,7 +5792,7 @@
       <c r="F165" s="11"/>
       <c r="G165" s="8"/>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="6"/>
       <c r="B166" s="7" t="s">
         <v>30</v>
@@ -5805,7 +5805,7 @@
       <c r="F166" s="11"/>
       <c r="G166" s="8"/>
     </row>
-    <row r="167" spans="1:7" ht="22" customHeight="1" thickBot="1">
+    <row r="167" spans="1:7" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="12"/>
       <c r="B167" s="19"/>
       <c r="C167" s="13"/>
@@ -5814,20 +5814,20 @@
       <c r="F167" s="13"/>
       <c r="G167" s="14"/>
     </row>
-    <row r="168" spans="1:7" ht="22" customHeight="1"/>
-    <row r="169" spans="1:7" ht="22" customHeight="1"/>
-    <row r="170" spans="1:7" ht="22" customHeight="1"/>
-    <row r="171" spans="1:7" ht="22" customHeight="1"/>
-    <row r="172" spans="1:7" ht="22" customHeight="1"/>
-    <row r="173" spans="1:7" ht="22" customHeight="1"/>
-    <row r="174" spans="1:7" ht="22" customHeight="1"/>
-    <row r="175" spans="1:7" ht="22" customHeight="1"/>
-    <row r="176" spans="1:7" ht="22" customHeight="1"/>
-    <row r="177" ht="22" customHeight="1"/>
-    <row r="178" ht="22" customHeight="1"/>
-    <row r="179" ht="22" customHeight="1"/>
-    <row r="180" ht="22" customHeight="1"/>
-    <row r="181" ht="22" customHeight="1"/>
+    <row r="168" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -5848,41 +5848,41 @@
       <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.83203125" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="24" customFormat="1" ht="30">
+    <row r="1" spans="1:7" s="24" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B1" s="24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="28">
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -5897,7 +5897,7 @@
       <c r="F9" s="50"/>
       <c r="G9" s="51"/>
     </row>
-    <row r="10" spans="1:7" ht="21" thickBot="1">
+    <row r="10" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="15">
         <v>1</v>
       </c>
@@ -5910,7 +5910,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" ht="20">
+    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
         <v>2</v>
       </c>
@@ -5923,7 +5923,7 @@
       <c r="F11" s="11"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="7" t="s">
         <v>1</v>
@@ -5934,7 +5934,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
         <v>0</v>
@@ -5945,7 +5945,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="7" t="s">
         <v>62</v>
@@ -5956,7 +5956,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="7" t="s">
         <v>63</v>
@@ -5967,7 +5967,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="7" t="s">
         <v>64</v>
@@ -5978,10 +5978,10 @@
       <c r="F16" s="11"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>65</v>
@@ -5991,10 +5991,10 @@
       <c r="F17" s="11"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="18">
+    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>66</v>
@@ -6004,7 +6004,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" s="32" customFormat="1">
+    <row r="19" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="B19" s="37"/>
       <c r="C19" s="10"/>
@@ -6013,7 +6013,7 @@
       <c r="F19" s="10"/>
       <c r="G19" s="31"/>
     </row>
-    <row r="20" spans="1:7" s="32" customFormat="1">
+    <row r="20" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
       <c r="B20" s="7"/>
       <c r="C20" s="10"/>
@@ -6022,7 +6022,7 @@
       <c r="F20" s="10"/>
       <c r="G20" s="31"/>
     </row>
-    <row r="21" spans="1:7" s="32" customFormat="1">
+    <row r="21" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="30"/>
       <c r="B21" s="33"/>
       <c r="C21" s="10"/>
@@ -6031,7 +6031,7 @@
       <c r="F21" s="10"/>
       <c r="G21" s="31"/>
     </row>
-    <row r="22" spans="1:7" s="32" customFormat="1">
+    <row r="22" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="7"/>
       <c r="C22" s="10"/>
@@ -6040,7 +6040,7 @@
       <c r="F22" s="10"/>
       <c r="G22" s="31"/>
     </row>
-    <row r="23" spans="1:7" s="32" customFormat="1">
+    <row r="23" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="30"/>
       <c r="B23" s="7"/>
       <c r="C23" s="10"/>
@@ -6049,7 +6049,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="31"/>
     </row>
-    <row r="24" spans="1:7" s="32" customFormat="1">
+    <row r="24" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="30"/>
       <c r="B24" s="7"/>
       <c r="C24" s="10"/>
@@ -6058,7 +6058,7 @@
       <c r="F24" s="10"/>
       <c r="G24" s="31"/>
     </row>
-    <row r="25" spans="1:7" s="32" customFormat="1">
+    <row r="25" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="30"/>
       <c r="B25" s="34"/>
       <c r="C25" s="10"/>
@@ -6067,7 +6067,7 @@
       <c r="F25" s="10"/>
       <c r="G25" s="31"/>
     </row>
-    <row r="26" spans="1:7" s="32" customFormat="1">
+    <row r="26" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="30"/>
       <c r="B26" s="7"/>
       <c r="C26" s="10"/>
@@ -6076,7 +6076,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="31"/>
     </row>
-    <row r="27" spans="1:7" s="32" customFormat="1">
+    <row r="27" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="30"/>
       <c r="B27" s="7"/>
       <c r="C27" s="10"/>
@@ -6085,7 +6085,7 @@
       <c r="F27" s="10"/>
       <c r="G27" s="31"/>
     </row>
-    <row r="28" spans="1:7" s="32" customFormat="1">
+    <row r="28" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="30"/>
       <c r="B28" s="7"/>
       <c r="C28" s="10"/>
@@ -6094,7 +6094,7 @@
       <c r="F28" s="10"/>
       <c r="G28" s="31"/>
     </row>
-    <row r="29" spans="1:7" s="32" customFormat="1">
+    <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="30"/>
       <c r="B29" s="7"/>
       <c r="C29" s="10"/>
@@ -6103,7 +6103,7 @@
       <c r="F29" s="10"/>
       <c r="G29" s="31"/>
     </row>
-    <row r="30" spans="1:7" s="32" customFormat="1">
+    <row r="30" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="30"/>
       <c r="B30" s="9"/>
       <c r="C30" s="10"/>
@@ -6112,7 +6112,7 @@
       <c r="F30" s="10"/>
       <c r="G30" s="31"/>
     </row>
-    <row r="31" spans="1:7" s="32" customFormat="1">
+    <row r="31" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="30"/>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -6121,7 +6121,7 @@
       <c r="F31" s="10"/>
       <c r="G31" s="31"/>
     </row>
-    <row r="32" spans="1:7" s="32" customFormat="1">
+    <row r="32" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="9"/>
       <c r="C32" s="35"/>
@@ -6130,7 +6130,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="31"/>
     </row>
-    <row r="33" spans="1:7" s="32" customFormat="1">
+    <row r="33" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="9" t="s">
         <v>67</v>
@@ -6141,7 +6141,7 @@
       <c r="F33" s="10"/>
       <c r="G33" s="31"/>
     </row>
-    <row r="34" spans="1:7" s="32" customFormat="1">
+    <row r="34" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="9" t="s">
         <v>68</v>
@@ -6158,7 +6158,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="32" customFormat="1">
+    <row r="35" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="9" t="s">
         <v>72</v>
@@ -6169,7 +6169,7 @@
       <c r="F35" s="10"/>
       <c r="G35" s="31"/>
     </row>
-    <row r="36" spans="1:7" s="32" customFormat="1">
+    <row r="36" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="30"/>
       <c r="B36" s="9" t="s">
         <v>73</v>
@@ -6180,7 +6180,7 @@
       <c r="F36" s="10"/>
       <c r="G36" s="31"/>
     </row>
-    <row r="37" spans="1:7" s="32" customFormat="1">
+    <row r="37" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30"/>
       <c r="B37" s="9" t="s">
         <v>74</v>
@@ -6191,7 +6191,7 @@
       <c r="F37" s="10"/>
       <c r="G37" s="31"/>
     </row>
-    <row r="38" spans="1:7" s="32" customFormat="1">
+    <row r="38" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
       <c r="B38" s="9" t="s">
         <v>75</v>
@@ -6202,7 +6202,7 @@
       <c r="F38" s="10"/>
       <c r="G38" s="31"/>
     </row>
-    <row r="39" spans="1:7" s="32" customFormat="1">
+    <row r="39" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
       <c r="B39" s="7"/>
       <c r="C39" s="10"/>
@@ -6211,7 +6211,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="31"/>
     </row>
-    <row r="40" spans="1:7" s="32" customFormat="1">
+    <row r="40" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="30"/>
       <c r="B40" s="34"/>
       <c r="C40" s="10"/>
@@ -6220,7 +6220,7 @@
       <c r="F40" s="10"/>
       <c r="G40" s="31"/>
     </row>
-    <row r="41" spans="1:7" s="32" customFormat="1">
+    <row r="41" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
       <c r="B41" s="7"/>
       <c r="C41" s="10"/>
@@ -6229,7 +6229,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="31"/>
     </row>
-    <row r="42" spans="1:7" s="32" customFormat="1">
+    <row r="42" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="34"/>
       <c r="C42" s="10"/>
@@ -6238,7 +6238,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="31"/>
     </row>
-    <row r="43" spans="1:7" s="32" customFormat="1">
+    <row r="43" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="7"/>
       <c r="C43" s="10"/>
@@ -6247,7 +6247,7 @@
       <c r="F43" s="10"/>
       <c r="G43" s="31"/>
     </row>
-    <row r="44" spans="1:7" s="32" customFormat="1">
+    <row r="44" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="7"/>
       <c r="C44" s="10"/>
@@ -6256,7 +6256,7 @@
       <c r="F44" s="10"/>
       <c r="G44" s="31"/>
     </row>
-    <row r="45" spans="1:7" s="32" customFormat="1">
+    <row r="45" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -6265,7 +6265,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="31"/>
     </row>
-    <row r="46" spans="1:7" s="32" customFormat="1">
+    <row r="46" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -6274,7 +6274,7 @@
       <c r="F46" s="10"/>
       <c r="G46" s="31"/>
     </row>
-    <row r="47" spans="1:7" s="32" customFormat="1">
+    <row r="47" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -6283,7 +6283,7 @@
       <c r="F47" s="10"/>
       <c r="G47" s="31"/>
     </row>
-    <row r="48" spans="1:7" s="32" customFormat="1">
+    <row r="48" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -6292,7 +6292,7 @@
       <c r="F48" s="10"/>
       <c r="G48" s="31"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -6301,7 +6301,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="11"/>
       <c r="C50" s="11"/>
@@ -6310,7 +6310,7 @@
       <c r="F50" s="11"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
@@ -6319,7 +6319,7 @@
       <c r="F51" s="11"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -6328,7 +6328,7 @@
       <c r="F52" s="11"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1">
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -6337,12 +6337,12 @@
       <c r="F53" s="13"/>
       <c r="G53" s="14"/>
     </row>
-    <row r="54" spans="1:7" ht="20">
+    <row r="54" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="15">
         <v>3</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C54" s="21"/>
       <c r="D54" s="21"/>
@@ -6350,10 +6350,10 @@
       <c r="F54" s="11"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C55" s="11" t="s">
         <v>76</v>
@@ -6363,7 +6363,7 @@
       <c r="F55" s="11"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="36"/>
       <c r="C56" s="11"/>
@@ -6372,7 +6372,7 @@
       <c r="F56" s="11"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="36"/>
       <c r="C57" s="11"/>
@@ -6381,7 +6381,7 @@
       <c r="F57" s="11"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="36"/>
       <c r="C58" s="11"/>
@@ -6390,7 +6390,7 @@
       <c r="F58" s="11"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="36"/>
       <c r="C59" s="11"/>
@@ -6399,7 +6399,7 @@
       <c r="F59" s="11"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15" thickBot="1">
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="36"/>
       <c r="C60" s="11"/>
@@ -6408,12 +6408,12 @@
       <c r="F60" s="11"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="20">
+    <row r="61" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A61" s="15">
         <v>4</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C61" s="21"/>
       <c r="D61" s="21"/>
@@ -6421,10 +6421,10 @@
       <c r="F61" s="21"/>
       <c r="G61" s="48"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
@@ -6432,7 +6432,7 @@
       <c r="F62" s="11"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="36"/>
       <c r="C63" s="11"/>
@@ -6441,7 +6441,7 @@
       <c r="F63" s="11"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="36"/>
       <c r="C64" s="11"/>
@@ -6450,7 +6450,7 @@
       <c r="F64" s="11"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="36"/>
       <c r="C65" s="11"/>
@@ -6459,7 +6459,7 @@
       <c r="F65" s="11"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="36"/>
       <c r="C66" s="11"/>
@@ -6468,7 +6468,7 @@
       <c r="F66" s="11"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="36"/>
       <c r="C67" s="11"/>
@@ -6477,7 +6477,7 @@
       <c r="F67" s="11"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="36"/>
       <c r="C68" s="11"/>
@@ -6486,7 +6486,7 @@
       <c r="F68" s="11"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="36"/>
       <c r="C69" s="11"/>
@@ -6495,7 +6495,7 @@
       <c r="F69" s="11"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="36"/>
       <c r="C70" s="11"/>
@@ -6504,7 +6504,7 @@
       <c r="F70" s="11"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="36"/>
       <c r="C71" s="11"/>
@@ -6513,7 +6513,7 @@
       <c r="F71" s="11"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
@@ -6521,10 +6521,10 @@
       <c r="F72" s="11"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
@@ -6532,7 +6532,7 @@
       <c r="F73" s="11"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
@@ -6540,7 +6540,7 @@
       <c r="F74" s="11"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="36"/>
       <c r="C75" s="11"/>
@@ -6549,7 +6549,7 @@
       <c r="F75" s="11"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="36"/>
       <c r="C76" s="11"/>
@@ -6558,10 +6558,10 @@
       <c r="F76" s="11"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
@@ -6569,10 +6569,10 @@
       <c r="F77" s="11"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
@@ -6580,10 +6580,10 @@
       <c r="F78" s="11"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
@@ -6591,7 +6591,7 @@
       <c r="F79" s="11"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="36"/>
       <c r="C80" s="11"/>
@@ -6600,7 +6600,7 @@
       <c r="F80" s="11"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="36"/>
       <c r="C81" s="11"/>
@@ -6609,7 +6609,7 @@
       <c r="F81" s="11"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="36"/>
       <c r="C82" s="11"/>
@@ -6618,7 +6618,7 @@
       <c r="F82" s="11"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
@@ -6626,7 +6626,7 @@
       <c r="F83" s="11"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="36"/>
       <c r="C84" s="11"/>
@@ -6635,7 +6635,7 @@
       <c r="F84" s="11"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="36"/>
       <c r="C85" s="11"/>
@@ -6644,7 +6644,7 @@
       <c r="F85" s="11"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
@@ -6652,33 +6652,33 @@
       <c r="F86" s="11"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15" thickBot="1">
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="20">
+    <row r="90" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A90" s="15">
         <v>5</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C90" s="21"/>
       <c r="D90" s="21"/>
@@ -6686,66 +6686,66 @@
       <c r="F90" s="21"/>
       <c r="G90" s="48"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
       <c r="F92" s="11"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="6"/>
       <c r="C99" s="11"/>
       <c r="D99" s="11"/>
@@ -6753,7 +6753,7 @@
       <c r="F99" s="11"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="6"/>
       <c r="B100" s="36"/>
       <c r="C100" s="11"/>
@@ -6762,7 +6762,7 @@
       <c r="F100" s="11"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="6"/>
       <c r="B101" s="36"/>
       <c r="C101" s="11"/>
@@ -6771,7 +6771,7 @@
       <c r="F101" s="11"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="6"/>
       <c r="B102" s="36"/>
       <c r="C102" s="11"/>
@@ -6780,7 +6780,7 @@
       <c r="F102" s="11"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="6"/>
       <c r="B103" s="36"/>
       <c r="C103" s="11"/>
@@ -6789,7 +6789,7 @@
       <c r="F103" s="11"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="6"/>
       <c r="B104" s="36"/>
       <c r="C104" s="11"/>
@@ -6798,7 +6798,7 @@
       <c r="F104" s="11"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="6"/>
       <c r="B105" s="36"/>
       <c r="C105" s="11"/>
@@ -6807,7 +6807,7 @@
       <c r="F105" s="11"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="6"/>
       <c r="B106" s="36"/>
       <c r="C106" s="11"/>
@@ -6816,10 +6816,10 @@
       <c r="F106" s="11"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="6"/>
       <c r="B107" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C107" s="11"/>
       <c r="D107" s="11"/>
@@ -6827,10 +6827,10 @@
       <c r="F107" s="11"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="6"/>
       <c r="B108" s="36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
@@ -6838,7 +6838,7 @@
       <c r="F108" s="11"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="6"/>
       <c r="B109" s="36"/>
       <c r="C109" s="11"/>
@@ -6847,7 +6847,7 @@
       <c r="F109" s="11"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="6"/>
       <c r="C110" s="11"/>
       <c r="D110" s="11"/>
@@ -6855,7 +6855,7 @@
       <c r="F110" s="11"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="6"/>
       <c r="B111" s="36"/>
       <c r="C111" s="11"/>
@@ -6864,7 +6864,7 @@
       <c r="F111" s="11"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="6"/>
       <c r="B112" s="36"/>
       <c r="C112" s="11"/>
@@ -6873,7 +6873,7 @@
       <c r="F112" s="11"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
       <c r="B113" s="36"/>
       <c r="C113" s="11"/>
@@ -6882,10 +6882,10 @@
       <c r="F113" s="11"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="42">
+    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="6"/>
       <c r="B114" s="47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C114" s="11"/>
       <c r="D114" s="11"/>
@@ -6893,7 +6893,7 @@
       <c r="F114" s="11"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
       <c r="C115" s="11"/>
       <c r="D115" s="11"/>
@@ -6901,7 +6901,7 @@
       <c r="F115" s="11"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="6"/>
       <c r="C116" s="11"/>
       <c r="D116" s="11"/>
@@ -6909,7 +6909,7 @@
       <c r="F116" s="11"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="6"/>
       <c r="C117" s="11"/>
       <c r="D117" s="11"/>
@@ -6917,7 +6917,7 @@
       <c r="F117" s="11"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="6"/>
       <c r="C118" s="11"/>
       <c r="D118" s="11"/>
@@ -6925,7 +6925,7 @@
       <c r="F118" s="11"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="6"/>
       <c r="C119" s="11"/>
       <c r="D119" s="11"/>
@@ -6933,7 +6933,7 @@
       <c r="F119" s="11"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="6"/>
       <c r="C120" s="11"/>
       <c r="D120" s="11"/>
@@ -6941,7 +6941,7 @@
       <c r="F120" s="11"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="6"/>
       <c r="C121" s="11"/>
       <c r="D121" s="11"/>
@@ -6949,7 +6949,7 @@
       <c r="F121" s="11"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="6"/>
       <c r="B122" s="36"/>
       <c r="C122" s="11"/>
@@ -6958,7 +6958,7 @@
       <c r="F122" s="11"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="6"/>
       <c r="B123" s="36"/>
       <c r="C123" s="11"/>
@@ -6967,7 +6967,7 @@
       <c r="F123" s="11"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="6"/>
       <c r="B124" s="36"/>
       <c r="C124" s="11"/>
@@ -6976,7 +6976,7 @@
       <c r="F124" s="11"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="6"/>
       <c r="B125" s="36"/>
       <c r="C125" s="11"/>
@@ -6985,7 +6985,7 @@
       <c r="F125" s="11"/>
       <c r="G125" s="8"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="6"/>
       <c r="B126" s="36"/>
       <c r="C126" s="11"/>
@@ -6994,7 +6994,7 @@
       <c r="F126" s="11"/>
       <c r="G126" s="8"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="6"/>
       <c r="B127" s="36"/>
       <c r="C127" s="11"/>
@@ -7003,10 +7003,10 @@
       <c r="F127" s="11"/>
       <c r="G127" s="8"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="6"/>
       <c r="B128" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C128" s="11"/>
       <c r="D128" s="11"/>
@@ -7014,7 +7014,7 @@
       <c r="F128" s="11"/>
       <c r="G128" s="8"/>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="6"/>
       <c r="B129" s="36"/>
       <c r="C129" s="11"/>
@@ -7023,7 +7023,7 @@
       <c r="F129" s="11"/>
       <c r="G129" s="8"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="6"/>
       <c r="B130" s="36"/>
       <c r="C130" s="11"/>
@@ -7032,7 +7032,7 @@
       <c r="F130" s="11"/>
       <c r="G130" s="8"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="6"/>
       <c r="B131" s="36"/>
       <c r="C131" s="11"/>
@@ -7041,7 +7041,7 @@
       <c r="F131" s="11"/>
       <c r="G131" s="8"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="6"/>
       <c r="B132" s="36"/>
       <c r="C132" s="11"/>
@@ -7050,7 +7050,7 @@
       <c r="F132" s="11"/>
       <c r="G132" s="8"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="6"/>
       <c r="B133" s="36"/>
       <c r="C133" s="11"/>
@@ -7059,7 +7059,7 @@
       <c r="F133" s="11"/>
       <c r="G133" s="8"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="6"/>
       <c r="B134" s="36"/>
       <c r="C134" s="11"/>
@@ -7068,7 +7068,7 @@
       <c r="F134" s="11"/>
       <c r="G134" s="8"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="6"/>
       <c r="B135" s="36"/>
       <c r="C135" s="11"/>
@@ -7077,7 +7077,7 @@
       <c r="F135" s="11"/>
       <c r="G135" s="8"/>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="6"/>
       <c r="B136" s="36"/>
       <c r="C136" s="11"/>
@@ -7086,7 +7086,7 @@
       <c r="F136" s="11"/>
       <c r="G136" s="8"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="6"/>
       <c r="B137" s="36"/>
       <c r="C137" s="11"/>
@@ -7095,7 +7095,7 @@
       <c r="F137" s="11"/>
       <c r="G137" s="8"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="6"/>
       <c r="B138" s="36"/>
       <c r="C138" s="11"/>
@@ -7104,7 +7104,7 @@
       <c r="F138" s="11"/>
       <c r="G138" s="8"/>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="6"/>
       <c r="B139" s="36"/>
       <c r="C139" s="11"/>
@@ -7113,7 +7113,7 @@
       <c r="F139" s="11"/>
       <c r="G139" s="8"/>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="6"/>
       <c r="B140" s="36"/>
       <c r="C140" s="11"/>
@@ -7122,7 +7122,7 @@
       <c r="F140" s="11"/>
       <c r="G140" s="8"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="6"/>
       <c r="B141" s="36"/>
       <c r="C141" s="11"/>
@@ -7131,7 +7131,7 @@
       <c r="F141" s="11"/>
       <c r="G141" s="8"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
       <c r="B142" s="36"/>
       <c r="C142" s="11"/>
@@ -7140,7 +7140,7 @@
       <c r="F142" s="11"/>
       <c r="G142" s="8"/>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="6"/>
       <c r="B143" s="36"/>
       <c r="C143" s="11"/>
@@ -7149,7 +7149,7 @@
       <c r="F143" s="11"/>
       <c r="G143" s="8"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="6"/>
       <c r="B144" s="36"/>
       <c r="C144" s="11"/>
@@ -7158,7 +7158,7 @@
       <c r="F144" s="11"/>
       <c r="G144" s="8"/>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="6"/>
       <c r="B145" s="36"/>
       <c r="C145" s="11"/>
@@ -7167,7 +7167,7 @@
       <c r="F145" s="11"/>
       <c r="G145" s="8"/>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="6"/>
       <c r="B146" s="36"/>
       <c r="C146" s="11"/>
@@ -7176,7 +7176,7 @@
       <c r="F146" s="11"/>
       <c r="G146" s="8"/>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="6"/>
       <c r="B147" s="36"/>
       <c r="C147" s="11"/>
@@ -7185,7 +7185,7 @@
       <c r="F147" s="11"/>
       <c r="G147" s="8"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="6"/>
       <c r="B148" s="36"/>
       <c r="C148" s="11"/>
@@ -7194,7 +7194,7 @@
       <c r="F148" s="11"/>
       <c r="G148" s="8"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="6"/>
       <c r="B149" s="36"/>
       <c r="C149" s="11"/>
@@ -7203,7 +7203,7 @@
       <c r="F149" s="11"/>
       <c r="G149" s="8"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="6"/>
       <c r="B150" s="36"/>
       <c r="C150" s="11"/>
@@ -7212,7 +7212,7 @@
       <c r="F150" s="11"/>
       <c r="G150" s="8"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="6"/>
       <c r="B151" s="36"/>
       <c r="C151" s="11"/>
@@ -7221,7 +7221,7 @@
       <c r="F151" s="11"/>
       <c r="G151" s="8"/>
     </row>
-    <row r="152" spans="1:7" ht="15" thickBot="1">
+    <row r="152" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
       <c r="B152" s="36"/>
       <c r="C152" s="11"/>
@@ -7230,12 +7230,12 @@
       <c r="F152" s="11"/>
       <c r="G152" s="8"/>
     </row>
-    <row r="153" spans="1:7" ht="20">
+    <row r="153" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A153" s="15">
         <v>6</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C153" s="21"/>
       <c r="D153" s="21"/>
@@ -7243,7 +7243,7 @@
       <c r="F153" s="21"/>
       <c r="G153" s="48"/>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="6"/>
       <c r="B154" s="36"/>
       <c r="C154" s="11"/>
@@ -7252,10 +7252,10 @@
       <c r="F154" s="11"/>
       <c r="G154" s="8"/>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="6"/>
       <c r="B155" s="36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11"/>
@@ -7263,10 +7263,10 @@
       <c r="F155" s="11"/>
       <c r="G155" s="8"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="6"/>
       <c r="B156" s="16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C156" s="11"/>
       <c r="D156" s="11"/>
@@ -7274,10 +7274,10 @@
       <c r="F156" s="11"/>
       <c r="G156" s="8"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="6"/>
       <c r="B157" s="38" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C157" s="11"/>
       <c r="D157" s="11"/>
@@ -7285,10 +7285,10 @@
       <c r="F157" s="11"/>
       <c r="G157" s="8"/>
     </row>
-    <row r="158" spans="1:7">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="6"/>
       <c r="B158" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C158" s="11"/>
       <c r="D158" s="11"/>
@@ -7296,10 +7296,10 @@
       <c r="F158" s="11"/>
       <c r="G158" s="8"/>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="6"/>
       <c r="B159" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C159" s="10"/>
       <c r="D159" s="11"/>
@@ -7307,7 +7307,7 @@
       <c r="F159" s="11"/>
       <c r="G159" s="8"/>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="6"/>
       <c r="B160" s="11"/>
       <c r="C160" s="11"/>
@@ -7316,7 +7316,7 @@
       <c r="F160" s="11"/>
       <c r="G160" s="8"/>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="6"/>
       <c r="B161" s="11"/>
       <c r="C161" s="11"/>
@@ -7325,7 +7325,7 @@
       <c r="F161" s="11"/>
       <c r="G161" s="8"/>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="6"/>
       <c r="B162" s="11"/>
       <c r="C162" s="11"/>
@@ -7334,7 +7334,7 @@
       <c r="F162" s="11"/>
       <c r="G162" s="8"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="6"/>
       <c r="B163" s="11"/>
       <c r="C163" s="11"/>
@@ -7343,7 +7343,7 @@
       <c r="F163" s="11"/>
       <c r="G163" s="8"/>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="6"/>
       <c r="B164" s="11"/>
       <c r="C164" s="11"/>
@@ -7352,7 +7352,7 @@
       <c r="F164" s="11"/>
       <c r="G164" s="8"/>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="6"/>
       <c r="B165" s="11"/>
       <c r="C165" s="11"/>
@@ -7361,7 +7361,7 @@
       <c r="F165" s="11"/>
       <c r="G165" s="8"/>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="6"/>
       <c r="B166" s="11"/>
       <c r="C166" s="11"/>
@@ -7370,7 +7370,7 @@
       <c r="F166" s="11"/>
       <c r="G166" s="8"/>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="6"/>
       <c r="B167" s="11"/>
       <c r="C167" s="11"/>
@@ -7379,7 +7379,7 @@
       <c r="F167" s="11"/>
       <c r="G167" s="8"/>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="6"/>
       <c r="B168" s="11"/>
       <c r="C168" s="11"/>
@@ -7388,7 +7388,7 @@
       <c r="F168" s="11"/>
       <c r="G168" s="8"/>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="6"/>
       <c r="B169" s="11"/>
       <c r="C169" s="11"/>
@@ -7397,7 +7397,7 @@
       <c r="F169" s="11"/>
       <c r="G169" s="8"/>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="6"/>
       <c r="B170" s="11"/>
       <c r="C170" s="11"/>
@@ -7406,7 +7406,7 @@
       <c r="F170" s="11"/>
       <c r="G170" s="8"/>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="6"/>
       <c r="B171" s="11"/>
       <c r="C171" s="11"/>
@@ -7415,7 +7415,7 @@
       <c r="F171" s="11"/>
       <c r="G171" s="8"/>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="6"/>
       <c r="B172" s="11"/>
       <c r="C172" s="11"/>
@@ -7424,7 +7424,7 @@
       <c r="F172" s="11"/>
       <c r="G172" s="8"/>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="6"/>
       <c r="B173" s="11"/>
       <c r="C173" s="11"/>
@@ -7433,7 +7433,7 @@
       <c r="F173" s="11"/>
       <c r="G173" s="8"/>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="6"/>
       <c r="B174" s="11"/>
       <c r="C174" s="11"/>
@@ -7442,7 +7442,7 @@
       <c r="F174" s="11"/>
       <c r="G174" s="8"/>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="6"/>
       <c r="B175" s="11"/>
       <c r="C175" s="11"/>
@@ -7451,7 +7451,7 @@
       <c r="F175" s="11"/>
       <c r="G175" s="8"/>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="6"/>
       <c r="B176" s="16"/>
       <c r="C176" s="11"/>
@@ -7460,7 +7460,7 @@
       <c r="F176" s="11"/>
       <c r="G176" s="8"/>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="6"/>
       <c r="B177" s="11"/>
       <c r="C177" s="11"/>
@@ -7469,7 +7469,7 @@
       <c r="F177" s="11"/>
       <c r="G177" s="8"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="6"/>
       <c r="B178" s="11"/>
       <c r="C178" s="11"/>
@@ -7478,7 +7478,7 @@
       <c r="F178" s="11"/>
       <c r="G178" s="8"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="6"/>
       <c r="B179" s="11"/>
       <c r="C179" s="11"/>
@@ -7487,7 +7487,7 @@
       <c r="F179" s="11"/>
       <c r="G179" s="8"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="6"/>
       <c r="B180" s="11"/>
       <c r="C180" s="11"/>
@@ -7496,7 +7496,7 @@
       <c r="F180" s="11"/>
       <c r="G180" s="8"/>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="6"/>
       <c r="B181" s="11"/>
       <c r="C181" s="11"/>
@@ -7505,7 +7505,7 @@
       <c r="F181" s="11"/>
       <c r="G181" s="8"/>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="6"/>
       <c r="B182" s="11"/>
       <c r="C182" s="11"/>
@@ -7514,7 +7514,7 @@
       <c r="F182" s="11"/>
       <c r="G182" s="8"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="6"/>
       <c r="B183" s="11"/>
       <c r="C183" s="11"/>
@@ -7523,7 +7523,7 @@
       <c r="F183" s="11"/>
       <c r="G183" s="8"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="6"/>
       <c r="B184" s="11"/>
       <c r="C184" s="11"/>
@@ -7532,10 +7532,10 @@
       <c r="F184" s="11"/>
       <c r="G184" s="8"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="6"/>
       <c r="B185" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C185" s="11"/>
       <c r="D185" s="11"/>
@@ -7543,7 +7543,7 @@
       <c r="F185" s="11"/>
       <c r="G185" s="8"/>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="6"/>
       <c r="B186" s="11"/>
       <c r="C186" s="11"/>
@@ -7552,7 +7552,7 @@
       <c r="F186" s="11"/>
       <c r="G186" s="8"/>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="6"/>
       <c r="B187" s="11"/>
       <c r="C187" s="11"/>
@@ -7561,7 +7561,7 @@
       <c r="F187" s="11"/>
       <c r="G187" s="8"/>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="6"/>
       <c r="B188" s="11"/>
       <c r="C188" s="11"/>
@@ -7570,7 +7570,7 @@
       <c r="F188" s="11"/>
       <c r="G188" s="8"/>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="6"/>
       <c r="B189" s="11"/>
       <c r="C189" s="11"/>
@@ -7579,7 +7579,7 @@
       <c r="F189" s="11"/>
       <c r="G189" s="8"/>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="6"/>
       <c r="B190" s="11"/>
       <c r="C190" s="11"/>
@@ -7588,7 +7588,7 @@
       <c r="F190" s="11"/>
       <c r="G190" s="8"/>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="6"/>
       <c r="B191" s="11"/>
       <c r="C191" s="11"/>
@@ -7597,7 +7597,7 @@
       <c r="F191" s="11"/>
       <c r="G191" s="8"/>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="6"/>
       <c r="B192" s="11"/>
       <c r="C192" s="11"/>
@@ -7606,7 +7606,7 @@
       <c r="F192" s="11"/>
       <c r="G192" s="8"/>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="6"/>
       <c r="B193" s="11"/>
       <c r="C193" s="11"/>
@@ -7615,7 +7615,7 @@
       <c r="F193" s="11"/>
       <c r="G193" s="8"/>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="6"/>
       <c r="B194" s="11"/>
       <c r="C194" s="11"/>
@@ -7624,7 +7624,7 @@
       <c r="F194" s="11"/>
       <c r="G194" s="8"/>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="6"/>
       <c r="B195" s="11"/>
       <c r="C195" s="11"/>
@@ -7633,7 +7633,7 @@
       <c r="F195" s="11"/>
       <c r="G195" s="8"/>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="6"/>
       <c r="B196" s="11"/>
       <c r="C196" s="11"/>
@@ -7642,7 +7642,7 @@
       <c r="F196" s="11"/>
       <c r="G196" s="8"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="6"/>
       <c r="B197" s="11"/>
       <c r="C197" s="11"/>
@@ -7651,7 +7651,7 @@
       <c r="F197" s="11"/>
       <c r="G197" s="8"/>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="6"/>
       <c r="B198" s="11"/>
       <c r="C198" s="11"/>
@@ -7660,7 +7660,7 @@
       <c r="F198" s="11"/>
       <c r="G198" s="8"/>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="6"/>
       <c r="B199" s="11"/>
       <c r="C199" s="11"/>
@@ -7669,7 +7669,7 @@
       <c r="F199" s="11"/>
       <c r="G199" s="8"/>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="6"/>
       <c r="B200" s="11"/>
       <c r="C200" s="11"/>
@@ -7678,7 +7678,7 @@
       <c r="F200" s="11"/>
       <c r="G200" s="8"/>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="6"/>
       <c r="B201" s="11"/>
       <c r="C201" s="11"/>
@@ -7687,7 +7687,7 @@
       <c r="F201" s="11"/>
       <c r="G201" s="8"/>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="6"/>
       <c r="B202" s="10"/>
       <c r="C202" s="11"/>
@@ -7696,7 +7696,7 @@
       <c r="F202" s="11"/>
       <c r="G202" s="8"/>
     </row>
-    <row r="203" spans="1:7" ht="15" customHeight="1">
+    <row r="203" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="6"/>
       <c r="B203" s="11"/>
       <c r="C203" s="11"/>
@@ -7705,7 +7705,7 @@
       <c r="F203" s="11"/>
       <c r="G203" s="8"/>
     </row>
-    <row r="204" spans="1:7" ht="15" customHeight="1" thickBot="1">
+    <row r="204" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="12"/>
       <c r="B204" s="13"/>
       <c r="C204" s="13"/>
@@ -7714,12 +7714,12 @@
       <c r="F204" s="13"/>
       <c r="G204" s="14"/>
     </row>
-    <row r="205" spans="1:7" ht="15" customHeight="1">
+    <row r="205" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="15">
         <v>7</v>
       </c>
       <c r="B205" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C205" s="21"/>
       <c r="D205" s="21"/>
@@ -7727,10 +7727,10 @@
       <c r="F205" s="21"/>
       <c r="G205" s="48"/>
     </row>
-    <row r="206" spans="1:7" ht="15" customHeight="1">
+    <row r="206" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="46"/>
       <c r="B206" s="36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C206" s="11"/>
       <c r="D206" s="11"/>
@@ -7738,10 +7738,10 @@
       <c r="F206" s="11"/>
       <c r="G206" s="8"/>
     </row>
-    <row r="207" spans="1:7" ht="15" customHeight="1">
+    <row r="207" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="46"/>
       <c r="B207" s="16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C207" s="11"/>
       <c r="D207" s="11"/>
@@ -7749,10 +7749,10 @@
       <c r="F207" s="11"/>
       <c r="G207" s="8"/>
     </row>
-    <row r="208" spans="1:7" ht="15" customHeight="1">
+    <row r="208" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="46"/>
       <c r="B208" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C208" s="11"/>
       <c r="D208" s="11"/>
@@ -7760,18 +7760,18 @@
       <c r="F208" s="11"/>
       <c r="G208" s="8"/>
     </row>
-    <row r="209" spans="1:7" ht="15" customHeight="1">
+    <row r="209" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="46"/>
       <c r="B209" s="11"/>
       <c r="C209" s="11"/>
       <c r="D209" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E209" s="11"/>
       <c r="F209" s="11"/>
       <c r="G209" s="8"/>
     </row>
-    <row r="210" spans="1:7" ht="15" customHeight="1">
+    <row r="210" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="46"/>
       <c r="B210" s="11"/>
       <c r="C210" s="11"/>
@@ -7780,7 +7780,7 @@
       <c r="F210" s="11"/>
       <c r="G210" s="8"/>
     </row>
-    <row r="211" spans="1:7" ht="15" customHeight="1">
+    <row r="211" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="46"/>
       <c r="B211" s="11"/>
       <c r="C211" s="11"/>
@@ -7789,7 +7789,7 @@
       <c r="F211" s="11"/>
       <c r="G211" s="8"/>
     </row>
-    <row r="212" spans="1:7" ht="15" customHeight="1">
+    <row r="212" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="46"/>
       <c r="B212" s="11"/>
       <c r="C212" s="11"/>
@@ -7798,7 +7798,7 @@
       <c r="F212" s="11"/>
       <c r="G212" s="8"/>
     </row>
-    <row r="213" spans="1:7" ht="15" customHeight="1">
+    <row r="213" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="46"/>
       <c r="B213" s="11"/>
       <c r="C213" s="11"/>
@@ -7807,7 +7807,7 @@
       <c r="F213" s="11"/>
       <c r="G213" s="8"/>
     </row>
-    <row r="214" spans="1:7" ht="15" customHeight="1">
+    <row r="214" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="46"/>
       <c r="B214" s="11"/>
       <c r="C214" s="11"/>
@@ -7816,7 +7816,7 @@
       <c r="F214" s="11"/>
       <c r="G214" s="8"/>
     </row>
-    <row r="215" spans="1:7" ht="15" customHeight="1">
+    <row r="215" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="46"/>
       <c r="B215" s="11"/>
       <c r="C215" s="11"/>
@@ -7825,7 +7825,7 @@
       <c r="F215" s="11"/>
       <c r="G215" s="8"/>
     </row>
-    <row r="216" spans="1:7" ht="15" customHeight="1">
+    <row r="216" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="46"/>
       <c r="B216" s="11"/>
       <c r="C216" s="11"/>
@@ -7834,7 +7834,7 @@
       <c r="F216" s="11"/>
       <c r="G216" s="8"/>
     </row>
-    <row r="217" spans="1:7" ht="15" customHeight="1">
+    <row r="217" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="6"/>
       <c r="B217" s="11"/>
       <c r="C217" s="11"/>
@@ -7843,7 +7843,7 @@
       <c r="F217" s="11"/>
       <c r="G217" s="8"/>
     </row>
-    <row r="218" spans="1:7" ht="15" customHeight="1">
+    <row r="218" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="6"/>
       <c r="B218" s="11"/>
       <c r="C218" s="11"/>
@@ -7852,7 +7852,7 @@
       <c r="F218" s="11"/>
       <c r="G218" s="8"/>
     </row>
-    <row r="219" spans="1:7" ht="15" customHeight="1">
+    <row r="219" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="6"/>
       <c r="B219" s="11"/>
       <c r="C219" s="11"/>
@@ -7861,7 +7861,7 @@
       <c r="F219" s="11"/>
       <c r="G219" s="8"/>
     </row>
-    <row r="220" spans="1:7" ht="15" customHeight="1">
+    <row r="220" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="6"/>
       <c r="B220" s="11"/>
       <c r="C220" s="11"/>
@@ -7870,7 +7870,7 @@
       <c r="F220" s="11"/>
       <c r="G220" s="8"/>
     </row>
-    <row r="221" spans="1:7" ht="15" customHeight="1">
+    <row r="221" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="6"/>
       <c r="B221" s="11"/>
       <c r="C221" s="11"/>
@@ -7879,7 +7879,7 @@
       <c r="F221" s="11"/>
       <c r="G221" s="8"/>
     </row>
-    <row r="222" spans="1:7" ht="15" customHeight="1">
+    <row r="222" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="6"/>
       <c r="B222" s="11"/>
       <c r="C222" s="11"/>
@@ -7888,7 +7888,7 @@
       <c r="F222" s="11"/>
       <c r="G222" s="8"/>
     </row>
-    <row r="223" spans="1:7" ht="15" customHeight="1">
+    <row r="223" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="6"/>
       <c r="B223" s="11"/>
       <c r="C223" s="11"/>
@@ -7897,7 +7897,7 @@
       <c r="F223" s="11"/>
       <c r="G223" s="8"/>
     </row>
-    <row r="224" spans="1:7" ht="15" customHeight="1">
+    <row r="224" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="6"/>
       <c r="B224" s="11"/>
       <c r="C224" s="11"/>
@@ -7906,7 +7906,7 @@
       <c r="F224" s="11"/>
       <c r="G224" s="8"/>
     </row>
-    <row r="225" spans="1:7" ht="15" customHeight="1">
+    <row r="225" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="6"/>
       <c r="B225" s="11"/>
       <c r="C225" s="11"/>
@@ -7915,7 +7915,7 @@
       <c r="F225" s="11"/>
       <c r="G225" s="8"/>
     </row>
-    <row r="226" spans="1:7" ht="15" customHeight="1">
+    <row r="226" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="6"/>
       <c r="B226" s="11"/>
       <c r="C226" s="11"/>
@@ -7924,7 +7924,7 @@
       <c r="F226" s="11"/>
       <c r="G226" s="8"/>
     </row>
-    <row r="227" spans="1:7" ht="15" customHeight="1">
+    <row r="227" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="6"/>
       <c r="B227" s="11"/>
       <c r="C227" s="11"/>
@@ -7933,7 +7933,7 @@
       <c r="F227" s="11"/>
       <c r="G227" s="8"/>
     </row>
-    <row r="228" spans="1:7" ht="15" customHeight="1" thickBot="1">
+    <row r="228" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="12"/>
       <c r="B228" s="13"/>
       <c r="C228" s="13"/>
@@ -7942,9 +7942,9 @@
       <c r="F228" s="13"/>
       <c r="G228" s="14"/>
     </row>
-    <row r="229" spans="1:7" ht="15" customHeight="1"/>
-    <row r="230" spans="1:7" ht="15" customHeight="1"/>
-    <row r="231" spans="1:7" ht="15" customHeight="1"/>
+    <row r="229" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C9:G9"/>
@@ -7964,30 +7964,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.83203125" customWidth="1"/>
-    <col min="4" max="4" width="44.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="94.5" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="94.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B1" s="24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28">
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -8002,7 +8002,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:7" ht="21" thickBot="1">
+    <row r="6" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -8015,7 +8015,7 @@
       <c r="F6" s="13"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="20">
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>2</v>
       </c>
@@ -8028,7 +8028,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="7" t="s">
         <v>1</v>
@@ -8039,7 +8039,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" ht="190" customHeight="1">
+    <row r="9" spans="1:7" ht="189.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="7" t="s">
         <v>0</v>
@@ -8050,7 +8050,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="16" t="s">
         <v>80</v>
@@ -8063,7 +8063,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7" ht="190.5" customHeight="1" thickBot="1">
+    <row r="11" spans="1:7" ht="190.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -8072,7 +8072,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:7" ht="20">
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>3</v>
       </c>
@@ -8085,7 +8085,7 @@
       <c r="F12" s="11"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="9" t="s">
         <v>82</v>
@@ -8098,7 +8098,7 @@
       <c r="F13" s="11"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="16" t="s">
         <v>84</v>
@@ -8109,7 +8109,7 @@
       <c r="F14" s="11"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="17"/>
       <c r="C15" s="11"/>
@@ -8118,7 +8118,7 @@
       <c r="F15" s="11"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7" ht="146.25" customHeight="1">
+    <row r="16" spans="1:7" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
@@ -8127,7 +8127,7 @@
       <c r="F16" s="11"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="36" t="s">
         <v>85</v>
@@ -8140,7 +8140,7 @@
       <c r="F17" s="11"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -8149,7 +8149,7 @@
       <c r="F18" s="11"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="180" customHeight="1" thickBot="1">
+    <row r="19" spans="1:7" ht="180" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -8158,7 +8158,7 @@
       <c r="F19" s="13"/>
       <c r="G19" s="14"/>
     </row>
-    <row r="20" spans="1:7" ht="20">
+    <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>4</v>
       </c>
@@ -8171,7 +8171,7 @@
       <c r="F20" s="11"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="16" t="s">
         <v>117</v>
@@ -8184,7 +8184,7 @@
       <c r="F21" s="11"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="214" customHeight="1">
+    <row r="22" spans="1:7" ht="213.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -8192,7 +8192,7 @@
       <c r="F22" s="11"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="16" t="s">
         <v>119</v>
@@ -8205,7 +8205,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="192" customHeight="1">
+    <row r="24" spans="1:7" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -8213,7 +8213,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="11" t="s">
         <v>121</v>
@@ -8226,7 +8226,7 @@
       <c r="F25" s="11"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="192.75" customHeight="1">
+    <row r="26" spans="1:7" ht="192.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -8235,7 +8235,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -8244,7 +8244,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15" thickBot="1">
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="19"/>
       <c r="C28" s="13"/>
@@ -8253,7 +8253,7 @@
       <c r="F28" s="13"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="1:7" ht="20">
+    <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>5</v>
       </c>
@@ -8266,7 +8266,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="16" t="s">
         <v>123</v>
@@ -8277,7 +8277,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="179.25" customHeight="1">
+    <row r="31" spans="1:7" ht="179.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" t="s">
         <v>124</v>
@@ -8288,7 +8288,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="16" t="s">
         <v>125</v>
@@ -8299,7 +8299,7 @@
       <c r="F32" s="11"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -8308,7 +8308,7 @@
       <c r="F33" s="11"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="16"/>
       <c r="C34" s="11"/>
@@ -8317,7 +8317,7 @@
       <c r="F34" s="11"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1">
+    <row r="35" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="B35" s="19"/>
       <c r="C35" s="13"/>
@@ -8326,7 +8326,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7" ht="20">
+    <row r="36" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>6</v>
       </c>
@@ -8339,7 +8339,7 @@
       <c r="F36" s="11"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="16" t="s">
         <v>90</v>
@@ -8352,7 +8352,7 @@
       <c r="F37" s="11"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="173.25" customHeight="1">
+    <row r="38" spans="1:7" ht="173.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
@@ -8360,7 +8360,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="18" customHeight="1">
+    <row r="39" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="16"/>
       <c r="C39" s="11"/>
@@ -8369,7 +8369,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="16" t="s">
         <v>91</v>
@@ -8382,7 +8382,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -8391,7 +8391,7 @@
       <c r="F41" s="11"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -8400,7 +8400,7 @@
       <c r="F42" s="11"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="153" customHeight="1">
+    <row r="43" spans="1:7" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -8409,7 +8409,7 @@
       <c r="F43" s="11"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="11" t="s">
         <v>94</v>
@@ -8420,7 +8420,7 @@
       <c r="F44" s="11"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -8429,7 +8429,7 @@
       <c r="F45" s="11"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -8438,7 +8438,7 @@
       <c r="F46" s="11"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -8447,7 +8447,7 @@
       <c r="F47" s="11"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1" thickBot="1">
+    <row r="48" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="19"/>
       <c r="C48" s="13"/>
@@ -8456,7 +8456,7 @@
       <c r="F48" s="13"/>
       <c r="G48" s="14"/>
     </row>
-    <row r="49" spans="1:7" ht="20">
+    <row r="49" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>7</v>
       </c>
@@ -8469,7 +8469,7 @@
       <c r="F49" s="11"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="16" t="s">
         <v>96</v>
@@ -8482,7 +8482,7 @@
       <c r="F50" s="11"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="16" t="s">
         <v>98</v>
@@ -8495,7 +8495,7 @@
       <c r="F51" s="11"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="192" customHeight="1">
+    <row r="52" spans="1:7" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="16"/>
       <c r="D52" s="11"/>
@@ -8503,7 +8503,7 @@
       <c r="F52" s="11"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="56" customHeight="1" thickBot="1">
+    <row r="53" spans="1:7" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="B53" s="19"/>
       <c r="C53" s="13"/>
@@ -8512,7 +8512,7 @@
       <c r="F53" s="13"/>
       <c r="G53" s="14"/>
     </row>
-    <row r="54" spans="1:7" ht="20">
+    <row r="54" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <v>8</v>
       </c>
@@ -8525,7 +8525,7 @@
       <c r="F54" s="11"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="16" t="s">
         <v>100</v>
@@ -8538,7 +8538,7 @@
       <c r="F55" s="11"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="16" t="s">
         <v>101</v>
@@ -8548,7 +8548,7 @@
       <c r="F56" s="11"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="16"/>
       <c r="D57" s="11"/>
@@ -8556,7 +8556,7 @@
       <c r="F57" s="11"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="154.5" customHeight="1">
+    <row r="58" spans="1:7" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -8565,7 +8565,7 @@
       <c r="F58" s="11"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="7" t="s">
         <v>127</v>
@@ -8578,7 +8578,7 @@
       <c r="F59" s="11"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="7" t="s">
         <v>129</v>
@@ -8591,7 +8591,7 @@
       <c r="F60" s="11"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="11" t="s">
         <v>102</v>
@@ -8604,7 +8604,7 @@
       <c r="F61" s="11"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11" t="s">
@@ -8615,7 +8615,7 @@
       <c r="F62" s="11"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -8624,7 +8624,7 @@
       <c r="F63" s="11"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="11"/>
       <c r="C64" s="11"/>
@@ -8633,7 +8633,7 @@
       <c r="F64" s="11"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
@@ -8642,7 +8642,7 @@
       <c r="F65" s="11"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="143" customHeight="1" thickBot="1">
+    <row r="66" spans="1:7" ht="143.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="19"/>
       <c r="C66" s="13"/>
@@ -8651,12 +8651,12 @@
       <c r="F66" s="13"/>
       <c r="G66" s="14"/>
     </row>
-    <row r="67" spans="1:7" ht="22" customHeight="1">
+    <row r="67" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="22" customHeight="1">
+    <row r="68" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>135</v>
       </c>
@@ -8664,7 +8664,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="22" customHeight="1">
+    <row r="69" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>136</v>
       </c>
@@ -8672,7 +8672,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="21.75" customHeight="1">
+    <row r="70" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>138</v>
       </c>
@@ -8680,8 +8680,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="187.5" customHeight="1"/>
-    <row r="72" spans="1:7" ht="22" customHeight="1">
+    <row r="71" spans="1:7" ht="187.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>140</v>
       </c>
@@ -8689,94 +8689,94 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="22" customHeight="1">
+    <row r="73" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
+        <v>201</v>
+      </c>
+      <c r="C73" t="s">
         <v>142</v>
       </c>
-      <c r="C73" t="s">
+    </row>
+    <row r="74" spans="1:7" ht="191.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="191.25" customHeight="1"/>
-    <row r="75" spans="1:7">
-      <c r="B75" t="s">
+    <row r="76" spans="1:7" ht="189" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>145</v>
-      </c>
-      <c r="C75" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="189" customHeight="1"/>
-    <row r="77" spans="1:7">
-      <c r="B77" t="s">
-        <v>146</v>
       </c>
       <c r="C77" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C78" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B79" s="44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C79" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="13" customFormat="1" ht="15" thickBot="1"/>
-    <row r="81" spans="2:3" ht="23">
+    <row r="80" spans="1:7" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="2:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B81" s="45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="83" spans="2:3">
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>150</v>
       </c>
-      <c r="C83" t="s">
+    </row>
+    <row r="84" spans="2:3" ht="186" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" ht="186" customHeight="1"/>
-    <row r="86" spans="2:3">
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>152</v>
       </c>
-      <c r="C86" t="s">
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>154</v>
+      </c>
+      <c r="C87" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="2:3">
-      <c r="B87" t="s">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>166</v>
+      </c>
+      <c r="C88" t="s">
         <v>155</v>
       </c>
-      <c r="C87" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3">
-      <c r="B88" t="s">
-        <v>167</v>
-      </c>
-      <c r="C88" t="s">
+    </row>
+    <row r="89" spans="2:3" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="46" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="89" spans="2:3" s="13" customFormat="1" ht="15" thickBot="1"/>
-    <row r="90" spans="2:3" ht="22" customHeight="1">
-      <c r="B90" s="46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>135</v>
       </c>
@@ -8784,7 +8784,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="2:3">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>136</v>
       </c>
@@ -8792,88 +8792,88 @@
         <v>137</v>
       </c>
     </row>
-    <row r="94" spans="2:3">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
+        <v>157</v>
+      </c>
+      <c r="C94" t="s">
         <v>158</v>
       </c>
-      <c r="C94" t="s">
+    </row>
+    <row r="95" spans="2:3" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="95" spans="2:3" ht="183.75" customHeight="1">
-      <c r="C95" t="s">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="96" spans="2:3">
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>161</v>
       </c>
-      <c r="C96" t="s">
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="97" spans="2:3">
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>163</v>
       </c>
-      <c r="C97" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3">
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C98" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="2:3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C99" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="100" spans="2:3" s="13" customFormat="1" ht="15" thickBot="1"/>
-    <row r="101" spans="2:3" ht="23">
+    <row r="100" spans="2:3" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="2:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B101" s="45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>149</v>
+      </c>
+      <c r="C103" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" ht="189" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>151</v>
+      </c>
+      <c r="C105" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="103" spans="2:3">
-      <c r="B103" t="s">
-        <v>150</v>
-      </c>
-      <c r="C103" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3" ht="189" customHeight="1"/>
-    <row r="105" spans="2:3">
-      <c r="B105" t="s">
-        <v>152</v>
-      </c>
-      <c r="C105" t="s">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>154</v>
+      </c>
+      <c r="C106" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="106" spans="2:3">
-      <c r="B106" t="s">
+      <c r="C107" t="s">
         <v>155</v>
-      </c>
-      <c r="C106" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="107" spans="2:3">
-      <c r="B107" t="s">
-        <v>167</v>
-      </c>
-      <c r="C107" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add SmartTemplate and Admin
</commit_message>
<xml_diff>
--- a/test/testcase/NORMAN Sanity Check.xlsx
+++ b/test/testcase/NORMAN Sanity Check.xlsx
@@ -4,13 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25365" windowHeight="14325" activeTab="3"/>
+    <workbookView xWindow="840" yWindow="900" windowWidth="19350" windowHeight="12930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisite" sheetId="6" r:id="rId1"/>
-    <sheet name="Auth - UIComposer - Project" sheetId="1" r:id="rId2"/>
-    <sheet name="DataModeler  DataSample Server" sheetId="2" r:id="rId3"/>
-    <sheet name="UserResearch" sheetId="5" r:id="rId4"/>
+    <sheet name="SmartTemplate" sheetId="8" r:id="rId2"/>
+    <sheet name="Auth - UIComposer - Project" sheetId="1" r:id="rId3"/>
+    <sheet name="DataModeler  DataSample Server" sheetId="2" r:id="rId4"/>
+    <sheet name="UserResearch" sheetId="5" r:id="rId5"/>
+    <sheet name="Admin" sheetId="10" r:id="rId6"/>
+    <sheet name="Admin_Users List" sheetId="11" r:id="rId7"/>
+    <sheet name="Admin_Audit" sheetId="12" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="271">
   <si>
     <t>New Project</t>
   </si>
@@ -682,6 +687,7 @@
         <sz val="14"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Sales Order Data model.xlsx</t>
@@ -707,6 +713,7 @@
         <sz val="14"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Sales Order Data model.xlsx</t>
@@ -754,12 +761,442 @@
   <si>
     <t>Select GLLinItems.zip (download from Jam here: https://jam4.sapjam.com/groups/60qDosrRAVDTLeeirVt451/content?folder_id=HuhlwTf9pwlyZHuNTugZ6J )</t>
   </si>
+  <si>
+    <t>git@github.wdf.sap.corp:Norman/Admin.git</t>
+  </si>
+  <si>
+    <t>Check DataBase name is the same name that norman DataBase i.e: norman</t>
+  </si>
+  <si>
+    <t>Open config-prod.json</t>
+  </si>
+  <si>
+    <t>Check port  is different that norman port: you can set 9001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clone  Admin: </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">create admin user: node server/createAdmin.js --name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>admin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --password </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Minisap1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --email </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>admin@sap.com</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">click in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UI Catalo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>g Menu</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">click on Upload icon </t>
+  </si>
+  <si>
+    <t>Set version 1.29.1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Select and Upload</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">select Type </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OpenUI5</t>
+    </r>
+  </si>
+  <si>
+    <t>select sapui5-dist-1.29.1-slagathor.zip and click on Open</t>
+  </si>
+  <si>
+    <t>when uploading is finished, click on close</t>
+  </si>
+  <si>
+    <t>logout of admin console</t>
+  </si>
+  <si>
+    <t>Log to ADMIN CONSOLE</t>
+  </si>
+  <si>
+    <t>Log to BUILD</t>
+  </si>
+  <si>
+    <r>
+      <t>log to admin with</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> administrator </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>user</t>
+    </r>
+  </si>
+  <si>
+    <t>no mandatory if you doesn't  use smartTemplate</t>
+  </si>
+  <si>
+    <t>https://jam4.sapjam.com/groups/60qDosrRAVDTLeeirVt451/documents/L44HAE1awt40FHsxOAqszJ</t>
+  </si>
+  <si>
+    <t>The 'Users' tab appears</t>
+  </si>
+  <si>
+    <t>Click on 'Back'</t>
+  </si>
+  <si>
+    <t>The 'Privacy statement' is opened in a new tab</t>
+  </si>
+  <si>
+    <t>Click on 'Privacy statement'</t>
+  </si>
+  <si>
+    <t>A pdf is opened in an other tab</t>
+  </si>
+  <si>
+    <t>Click on 'Help'</t>
+  </si>
+  <si>
+    <t>Help &amp; Provacy statement</t>
+  </si>
+  <si>
+    <t>Check that the tab is selected, you see users, the help…</t>
+  </si>
+  <si>
+    <t>You see this page :</t>
+  </si>
+  <si>
+    <t>you are connected</t>
+  </si>
+  <si>
+    <t>Enter your email address and your password</t>
+  </si>
+  <si>
+    <t>An error appears</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Enter a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wrong email address with password</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Enter a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> email address without password</t>
+    </r>
+  </si>
+  <si>
+    <t>Log In</t>
+  </si>
+  <si>
+    <t>The 'Guest' role appears in the details user</t>
+  </si>
+  <si>
+    <t>Click on 'OK'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the 'guest' is selected. </t>
+  </si>
+  <si>
+    <t>Select 'Guest' role</t>
+  </si>
+  <si>
+    <t>the 'Set Role' appears</t>
+  </si>
+  <si>
+    <t>Click on 'Pete Sampras' user</t>
+  </si>
+  <si>
+    <t>Search 'Pete Sampras'</t>
+  </si>
+  <si>
+    <t>User Role</t>
+  </si>
+  <si>
+    <t>Check that the pagination works well</t>
+  </si>
+  <si>
+    <t>Play with the pagination</t>
+  </si>
+  <si>
+    <t>Check that the name, the role and the address mail appear</t>
+  </si>
+  <si>
+    <t>the users appears with users details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on the icon detail </t>
+  </si>
+  <si>
+    <t>Users List</t>
+  </si>
+  <si>
+    <t>the users appears</t>
+  </si>
+  <si>
+    <t>Clear the search clicking on the cross</t>
+  </si>
+  <si>
+    <t>no user</t>
+  </si>
+  <si>
+    <t>Type 'dddd'</t>
+  </si>
+  <si>
+    <t>Pete Sampras appears</t>
+  </si>
+  <si>
+    <t>Type 'Pete'</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Sanity Check Users List</t>
+  </si>
+  <si>
+    <t>An error message appears</t>
+  </si>
+  <si>
+    <t>Click on 'Download'</t>
+  </si>
+  <si>
+    <t>Select end date : an old date</t>
+  </si>
+  <si>
+    <t>Select start date : an old date</t>
+  </si>
+  <si>
+    <t>The custom button is selected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select 'Custom' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check the data </t>
+  </si>
+  <si>
+    <r>
+      <t>Open the file downlo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ded file </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The file is downlo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ded</t>
+    </r>
+  </si>
+  <si>
+    <t>Select 'Last 24 Hours' and click on 'Download'</t>
+  </si>
+  <si>
+    <t>The 'Audit' page appears</t>
+  </si>
+  <si>
+    <t>Go to the 'Audit' tab</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -827,6 +1264,7 @@
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -858,6 +1296,7 @@
       <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -872,10 +1311,35 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1098,7 +1562,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1195,6 +1659,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="64" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1275,6 +1748,66 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1924050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1543050" y="371475"/>
+          <a:ext cx="381000" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2027,7 +2560,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2934,7 +3467,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3770,6 +4303,582 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2371725" cy="1251744"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="1143000"/>
+          <a:ext cx="2371725" cy="1251744"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3352800" cy="1994934"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1876426" y="1381125"/>
+          <a:ext cx="3352800" cy="1994934"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2095500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5866072" cy="2933036"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1876425" y="1524000"/>
+          <a:ext cx="5866072" cy="2933036"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3057526</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>37494</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3305174" cy="3190521"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438401" y="2323494"/>
+          <a:ext cx="3305174" cy="3190521"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1695450</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2371429" cy="1561905"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2143125" y="2476500"/>
+          <a:ext cx="2371429" cy="1561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>72909</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3448050" cy="3383419"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095500" y="2549409"/>
+          <a:ext cx="3448050" cy="3383419"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6754866" cy="2304601"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1876425" y="1314449"/>
+          <a:ext cx="6754866" cy="2304601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7610475" cy="2123810"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1933575" y="1390650"/>
+          <a:ext cx="7610475" cy="2123810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>92487</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3435814" cy="2822164"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2009776" y="1616487"/>
+          <a:ext cx="3435814" cy="2822164"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6452359" cy="2686050"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943100" y="1971676"/>
+          <a:ext cx="6452359" cy="2686050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3661947" cy="3113972"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2028825" y="2781300"/>
+          <a:ext cx="3661947" cy="3113972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2543174" cy="1417289"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828801" y="3238500"/>
+          <a:ext cx="2543174" cy="1417289"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="563616" cy="18601"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1876425" y="1314449"/>
+          <a:ext cx="563616" cy="18601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5762625" cy="2569632"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1943100" y="1257300"/>
+          <a:ext cx="5762625" cy="2569632"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>37602</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4048125" cy="2854717"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2019300" y="1371102"/>
+          <a:ext cx="4048125" cy="2854717"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7991475" cy="2277232"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="1524001"/>
+          <a:ext cx="7991475" cy="2277232"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3765947" cy="2126652"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2019300" y="2362200"/>
+          <a:ext cx="3765947" cy="2126652"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4057,15 +5166,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="76.7109375" customWidth="1"/>
+    <col min="2" max="2" width="101.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5" x14ac:dyDescent="0.5">
@@ -4164,10 +5273,112 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="42"/>
     </row>
+    <row r="16" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="18">
+        <v>1</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="39">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="39">
+        <v>1.2</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="39">
+        <v>1.3</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="39">
+        <v>1.4</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="22">
+        <v>2</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="22">
+        <v>3</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="39">
+        <v>3.1</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="39">
+        <v>3.2</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="39">
+        <v>3.3</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="55">
+        <v>3.4</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="55">
+        <v>3.5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B17" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
@@ -4180,10 +5391,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="56" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5840,7 +7130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G231"/>
   <sheetViews>
@@ -7960,11 +9250,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView topLeftCell="A65" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
@@ -8886,4 +10176,537 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B1" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>5</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="3">
+        <v>6</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="258.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>7</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" ht="276.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>8</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>9</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" ht="141" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="117" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B1" s="24" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="197.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="237" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3">
+        <v>5</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>245</v>
+      </c>
+      <c r="C13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="3">
+        <v>8</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>239</v>
+      </c>
+      <c r="C17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="121.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B1" s="24" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="230.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="186" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update Sanity check with smartTemplate
</commit_message>
<xml_diff>
--- a/test/testcase/NORMAN Sanity Check.xlsx
+++ b/test/testcase/NORMAN Sanity Check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="960" windowWidth="19350" windowHeight="12870" activeTab="1"/>
+    <workbookView xWindow="840" yWindow="1020" windowWidth="19350" windowHeight="12810" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisite" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="313">
   <si>
     <t>New Project</t>
   </si>
@@ -862,9 +862,6 @@
     <t xml:space="preserve">click on Upload icon </t>
   </si>
   <si>
-    <t>Set version 1.29.1</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">click on </t>
     </r>
@@ -907,9 +904,6 @@
     </r>
   </si>
   <si>
-    <t>select sapui5-dist-1.29.1-slagathor.zip and click on Open</t>
-  </si>
-  <si>
     <t>when uploading is finished, click on close</t>
   </si>
   <si>
@@ -1195,9 +1189,6 @@
     <t>create new project</t>
   </si>
   <si>
-    <t>open the project and click on View all: Map</t>
-  </si>
-  <si>
     <t>Click on add page</t>
   </si>
   <si>
@@ -1210,46 +1201,147 @@
     <t>click on the new page to open it</t>
   </si>
   <si>
-    <t>in the property pane, at the children level, add a smartFilterBar</t>
-  </si>
-  <si>
     <t>in the property pane, at the children level, Add Filter</t>
   </si>
   <si>
-    <t>select the Filter element</t>
-  </si>
-  <si>
     <t>Add tables</t>
   </si>
   <si>
-    <t>Add column</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>select Object page</t>
-  </si>
-  <si>
     <t>Add ObjectPageHeader</t>
   </si>
   <si>
-    <t>Add Section</t>
-  </si>
-  <si>
-    <t>In OUTLINE part select Section</t>
-  </si>
-  <si>
-    <t>ADD tables</t>
-  </si>
-  <si>
-    <t>ADD ContactTables</t>
-  </si>
-  <si>
-    <t>ADD multiGroupForms</t>
-  </si>
-  <si>
-    <t>ADD simpleForms</t>
+    <t>Set version 1.31.0</t>
+  </si>
+  <si>
+    <t>select sapui5-dist-1.31.0-slagathor.zip and click on Open</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">open the project and click on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Go to the Data Model</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Click on Import: select the file </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SmarTemplate demo data.xlsx, and open it</t>
+    </r>
+  </si>
+  <si>
+    <t>Check data model appears in the canvas</t>
+  </si>
+  <si>
+    <t>click on prototype page icon</t>
+  </si>
+  <si>
+    <t>in the property panel, at the children level, add a smartFilterBar</t>
+  </si>
+  <si>
+    <t>Select a main entity: "SalesOrder"</t>
+  </si>
+  <si>
+    <t>select the Filter element, bind Filter with Name</t>
+  </si>
+  <si>
+    <t>Add 3 columns</t>
+  </si>
+  <si>
+    <t>first column set Title: ID and bind Value ID</t>
+  </si>
+  <si>
+    <t>first column set Title: Name and bind Value Name</t>
+  </si>
+  <si>
+    <t>first column set Title:Status and bind Value Status</t>
+  </si>
+  <si>
+    <t>Click on Preview</t>
+  </si>
+  <si>
+    <t>Click on go</t>
+  </si>
+  <si>
+    <t>Check data appears in the table</t>
+  </si>
+  <si>
+    <t>Click on Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">click on </t>
+  </si>
+  <si>
+    <t>click on add page</t>
+  </si>
+  <si>
+    <t>add Object page</t>
+  </si>
+  <si>
+    <t>open Object Page</t>
+  </si>
+  <si>
+    <t>In outline part page 2 is selected</t>
+  </si>
+  <si>
+    <t>Select Main Entity: SalesOrder</t>
+  </si>
+  <si>
+    <t>In OUTLINE part select ObjectPageheader</t>
+  </si>
+  <si>
+    <t>do a binding on</t>
+  </si>
+  <si>
+    <t>Title: ID</t>
+  </si>
+  <si>
+    <t>description:Name</t>
+  </si>
+  <si>
+    <t>headerBarText:Status</t>
+  </si>
+  <si>
+    <t>In outline part</t>
+  </si>
+  <si>
+    <t>select page 1</t>
+  </si>
+  <si>
+    <t>click on Preview</t>
+  </si>
+  <si>
+    <t>click on Go</t>
+  </si>
+  <si>
+    <t>select the first line of the table</t>
+  </si>
+  <si>
+    <t>check you navigate on the page2</t>
+  </si>
+  <si>
+    <t>click on back</t>
+  </si>
+  <si>
+    <t>check you navigate on the page2, and hearder information are updated</t>
   </si>
 </sst>
 </file>
@@ -1738,15 +1830,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="64" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1757,6 +1840,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Bad" xfId="66" builtinId="27"/>
@@ -1881,6 +1973,446 @@
         <a:xfrm>
           <a:off x="1543050" y="371475"/>
           <a:ext cx="381000" cy="438150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1876425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3067050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1876425" y="3571875"/>
+          <a:ext cx="1190625" cy="600075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3419475</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>149962</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3419475" y="4819650"/>
+          <a:ext cx="1397737" cy="4162425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1943100</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3248025</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1943100" y="8924925"/>
+          <a:ext cx="1304925" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1657350</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1219200" y="9639300"/>
+          <a:ext cx="438150" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5400675" y="8496300"/>
+          <a:ext cx="9715500" cy="2019300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1857375</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3019425</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1857375" y="10306050"/>
+          <a:ext cx="1162050" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1847850</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="981075" y="10782300"/>
+          <a:ext cx="866775" cy="638175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3390900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>16385</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3390900" y="10306050"/>
+          <a:ext cx="2511935" cy="6048375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5263,8 +5795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5459,7 +5991,7 @@
         <v>207</v>
       </c>
       <c r="C26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -5486,10 +6018,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5499,12 +6031,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -5519,174 +6051,277 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A13" s="53" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="54" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="54" t="s">
+        <v>280</v>
+      </c>
+      <c r="B17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="54" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="54"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="54"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="54"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="54"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="54" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="B23" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="54"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="54" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>273</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="54" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="55" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="54" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="54" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="54" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="54" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="54" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="54" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="54"/>
+    </row>
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="54"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="54" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="54" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="54" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="54" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="58" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="57" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="57" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
-        <v>273</v>
-      </c>
-      <c r="B30" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="57"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="57" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="57" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="57" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="57" t="s">
-        <v>290</v>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="54" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="54" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="54" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="54" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="54" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>309</v>
+      </c>
+      <c r="B90" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>309</v>
+      </c>
+      <c r="B92" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5694,7 +6329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView topLeftCell="A89" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
@@ -7401,13 +8036,13 @@
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="56"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="60"/>
     </row>
     <row r="10" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="15">
@@ -10446,7 +11081,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="11"/>
@@ -10459,10 +11094,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -10474,10 +11109,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -10489,10 +11124,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -10503,7 +11138,7 @@
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -10515,7 +11150,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -10528,7 +11163,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="11"/>
@@ -10541,10 +11176,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -10556,10 +11191,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -10571,10 +11206,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -10614,7 +11249,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B1" s="24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -10642,7 +11277,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="11"/>
@@ -10655,10 +11290,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -10670,10 +11305,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="237" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10681,10 +11316,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -10692,7 +11327,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="11"/>
@@ -10705,15 +11340,15 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10721,10 +11356,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -10732,7 +11367,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="11"/>
@@ -10745,7 +11380,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10753,10 +11388,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C16" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -10764,10 +11399,10 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C17" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="117" customHeight="1" x14ac:dyDescent="0.25">
@@ -10775,10 +11410,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C18" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -10804,7 +11439,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B1" s="24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -10832,7 +11467,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="11"/>
@@ -10845,10 +11480,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -10860,10 +11495,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="186" customHeight="1" x14ac:dyDescent="0.25">
@@ -10871,10 +11506,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -10882,10 +11517,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -10893,7 +11528,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -10901,7 +11536,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.25">
@@ -10909,10 +11544,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File for DataBinding test
</commit_message>
<xml_diff>
--- a/test/testcase/NORMAN Sanity Check.xlsx
+++ b/test/testcase/NORMAN Sanity Check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1020" windowWidth="25440" windowHeight="15990" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="840" yWindow="1020" windowWidth="25440" windowHeight="15990" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisite" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="388">
   <si>
     <t>New Project</t>
   </si>
@@ -888,22 +888,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">select Type </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>OpenUI5</t>
-    </r>
-  </si>
-  <si>
     <t>when uploading is finished, click on close</t>
   </si>
   <si>
@@ -1198,13 +1182,7 @@
     <t>check 3 pages appear: Blank Page, ObjectPage, ListReport</t>
   </si>
   <si>
-    <t>Add ObjectPageHeader</t>
-  </si>
-  <si>
     <t>Set version 1.31.0</t>
-  </si>
-  <si>
-    <t>select sapui5-dist-1.31.0-slagathor.zip and click on Open</t>
   </si>
   <si>
     <r>
@@ -1245,15 +1223,9 @@
     <t>click on prototype page icon</t>
   </si>
   <si>
-    <t>in the property panel, at the children level, add a smartFilterBar</t>
-  </si>
-  <si>
     <t>Select a main entity: "SalesOrder"</t>
   </si>
   <si>
-    <t>first column set Title: ID and bind Value ID</t>
-  </si>
-  <si>
     <t>Click on Preview</t>
   </si>
   <si>
@@ -1270,24 +1242,6 @@
   </si>
   <si>
     <t>click on add page</t>
-  </si>
-  <si>
-    <t>add Object page</t>
-  </si>
-  <si>
-    <t>open Object Page</t>
-  </si>
-  <si>
-    <t>In outline part page 2 is selected</t>
-  </si>
-  <si>
-    <t>Select Main Entity: SalesOrder</t>
-  </si>
-  <si>
-    <t>In OUTLINE part select ObjectPageheader</t>
-  </si>
-  <si>
-    <t>do a binding on</t>
   </si>
   <si>
     <t>Title: ID</t>
@@ -1766,27 +1720,6 @@
     <t>In Outline part, select page1</t>
   </si>
   <si>
-    <t>in the property panel, at the children level, Add Filter</t>
-  </si>
-  <si>
-    <t>In Outline part select the Filter element, bind Filter with Name</t>
-  </si>
-  <si>
-    <t>in the property panel, Add tables</t>
-  </si>
-  <si>
-    <t>In outline part select Tables</t>
-  </si>
-  <si>
-    <t>in the property panel Add 3 columns</t>
-  </si>
-  <si>
-    <t>second column set Title: Name and bind Value Name</t>
-  </si>
-  <si>
-    <t>Third column set Title:Status and bind Value Status</t>
-  </si>
-  <si>
     <t>In List report page</t>
   </si>
   <si>
@@ -1899,6 +1832,117 @@
   </si>
   <si>
     <t>5,7</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">select Type </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SAPUI5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sapui5-dist-1.31.0-20150623.062420-9-opt-static.zip </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and click on Open</t>
+    </r>
+  </si>
+  <si>
+    <t>in the properties panel, at the children level, add a smartFilterBar</t>
+  </si>
+  <si>
+    <t>In OUTLINE part Select smartFilterBar</t>
+  </si>
+  <si>
+    <t>in the properties panel, at the children level, Add Filter</t>
+  </si>
+  <si>
+    <t>In properties part click on binding icon to  bind Filter with Name</t>
+  </si>
+  <si>
+    <t>In Outline part select the Filter element</t>
+  </si>
+  <si>
+    <t>in the properties panel, Add table</t>
+  </si>
+  <si>
+    <t>In outline part select Table</t>
+  </si>
+  <si>
+    <t>in the properties part under Children panel Add 3 columns</t>
+  </si>
+  <si>
+    <t>In outline part select Column</t>
+  </si>
+  <si>
+    <t>for first column set Title: ID and bind Value ID</t>
+  </si>
+  <si>
+    <t>for second column set Title: Name and bind Value Name</t>
+  </si>
+  <si>
+    <t>for Third column set Title:Status and bind Value Status</t>
+  </si>
+  <si>
+    <t>check 2 pages appear: ObjectPage, ListReport</t>
+  </si>
+  <si>
+    <t>Select  Object page</t>
+  </si>
+  <si>
+    <t>double click on page 2  to open Object Page</t>
+  </si>
+  <si>
+    <t>Check in outline part page 2 is selected</t>
+  </si>
+  <si>
+    <t>In DATA part Select Main Entity: SalesOrder</t>
+  </si>
+  <si>
+    <t>Add ObjectPageHeaders</t>
+  </si>
+  <si>
+    <t>In OUTLINE part select ObjectPageheaders</t>
+  </si>
+  <si>
+    <t>In properties page do a binding on</t>
+  </si>
+  <si>
+    <t>3,20</t>
+  </si>
+  <si>
+    <t>3,21</t>
+  </si>
+  <si>
+    <t>3,22</t>
   </si>
 </sst>
 </file>
@@ -2471,6 +2515,7 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2480,7 +2525,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Bad" xfId="66" builtinId="27"/>
@@ -6345,13 +6389,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1943100</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3248025</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6400,13 +6444,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1657350</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6455,13 +6499,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6510,13 +6554,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1857375</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3019425</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6565,13 +6609,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6620,13 +6664,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3714750</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>454535</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:colOff>292610</xdr:colOff>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7293,7 +7337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7328,7 +7372,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7627,7 +7671,7 @@
         <v>3.5</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -7743,7 +7787,7 @@
         <v>207</v>
       </c>
       <c r="C27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -7758,19 +7802,19 @@
     <row r="31" spans="1:3" s="67" customFormat="1" ht="53.1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A31" s="66"/>
       <c r="B31" s="67" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="67" customFormat="1" ht="53.1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A32" s="66"/>
       <c r="B32" s="67" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="67" customFormat="1" ht="53.1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A33" s="66"/>
       <c r="B33" s="67" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -7804,7 +7848,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="64" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="64" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="35.1" x14ac:dyDescent="0.45">
@@ -8052,7 +8096,7 @@
       <c r="F26" s="11"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -8061,7 +8105,7 @@
       <c r="F27" s="11"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -8070,7 +8114,7 @@
       <c r="F28" s="11"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -8079,7 +8123,7 @@
       <c r="F29" s="11"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -8088,7 +8132,7 @@
       <c r="F30" s="11"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -8097,7 +8141,7 @@
       <c r="F31" s="11"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -9469,7 +9513,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="64" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="64" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="24" customFormat="1" ht="35.1" x14ac:dyDescent="0.45">
@@ -9504,13 +9548,13 @@
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="77"/>
     </row>
     <row r="11" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
@@ -11592,7 +11636,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="64" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="64" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="35.1" x14ac:dyDescent="0.45">
@@ -12525,12 +12569,12 @@
   <sheetData>
     <row r="1" spans="1:6" s="65" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="65" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="35.1" x14ac:dyDescent="0.45">
       <c r="B2" s="24" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.45">
@@ -12557,7 +12601,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -12565,7 +12609,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.2">
@@ -12573,7 +12617,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12581,7 +12625,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12589,7 +12633,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12597,27 +12641,27 @@
         <v>6</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="58" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="59" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="57"/>
       <c r="B14" s="60" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="E14" s="60" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="383.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12627,45 +12671,45 @@
     </row>
     <row r="16" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="60" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="C16" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="383.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="60" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="C17" s="60" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="58" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="61"/>
       <c r="B19" s="62" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="57"/>
       <c r="B20" s="57" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="57"/>
       <c r="B21" s="60" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="C21" s="60" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="D21" s="60" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="E21" s="60" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="269.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12677,13 +12721,13 @@
     <row r="23" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="57"/>
       <c r="B23" s="60" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="D23" s="60" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12963,20 +13007,20 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="65" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="65" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.95" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -12985,13 +13029,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="71" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13009,16 +13053,16 @@
     <row r="7" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
     </row>
-    <row r="8" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="11" t="s">
-        <v>211</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13027,22 +13071,22 @@
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="11" t="s">
-        <v>275</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="13" customFormat="1" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.95" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -13051,7 +13095,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="73" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13059,7 +13103,7 @@
         <v>2.1</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -13067,7 +13111,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B17" s="68" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -13075,7 +13119,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -13083,10 +13127,10 @@
         <v>2.4</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13094,7 +13138,7 @@
         <v>2.5</v>
       </c>
       <c r="B20" s="68" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13116,10 +13160,10 @@
         <v>2.6</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13127,7 +13171,7 @@
         <v>2.7</v>
       </c>
       <c r="B26" s="53" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
@@ -13135,322 +13179,351 @@
         <v>3</v>
       </c>
       <c r="B27" s="73" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="74" t="s">
+        <v>326</v>
+      </c>
+      <c r="B28" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="74" t="s">
+        <v>327</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="74" t="s">
+        <v>328</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="74" t="s">
+        <v>329</v>
+      </c>
+      <c r="B31" s="54" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="74" t="s">
+        <v>330</v>
+      </c>
+      <c r="B32" s="54" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="56" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="74" t="s">
+        <v>331</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="74" t="s">
+        <v>332</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="74" t="s">
+        <v>333</v>
+      </c>
+      <c r="B35" s="53" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="74" t="s">
+        <v>334</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="74" t="s">
+        <v>335</v>
+      </c>
+      <c r="B37" s="53" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="74" t="s">
+        <v>336</v>
+      </c>
+      <c r="B38" s="53" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="74" t="s">
+        <v>337</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="74" t="s">
+        <v>338</v>
+      </c>
+      <c r="B40" s="53" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="74" t="s">
+        <v>339</v>
+      </c>
+      <c r="B41" s="53" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="74" t="s">
+        <v>340</v>
+      </c>
+      <c r="B42" s="53" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="74" t="s">
+        <v>341</v>
+      </c>
+      <c r="B43" s="53" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="53"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="74" t="s">
+        <v>342</v>
+      </c>
+      <c r="B54" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="74" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="77" t="s">
+      <c r="B57" t="s">
+        <v>279</v>
+      </c>
+      <c r="C57" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="74" t="s">
         <v>344</v>
       </c>
-      <c r="B28" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="77" t="s">
+      <c r="B61" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="74" t="s">
+        <v>385</v>
+      </c>
+      <c r="B63" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="53" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="74" t="s">
+        <v>386</v>
+      </c>
+      <c r="B70" s="53" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="74" t="s">
+        <v>387</v>
+      </c>
+      <c r="B71" s="53" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="53"/>
+    </row>
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="53"/>
+    </row>
+    <row r="74" spans="1:2" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A74" s="70">
+        <v>4</v>
+      </c>
+      <c r="B74" s="73" t="s">
         <v>345</v>
       </c>
-      <c r="B29" s="53" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="77" t="s">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="74" t="s">
         <v>346</v>
       </c>
-      <c r="B30" s="53" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="77" t="s">
+      <c r="B75" s="53" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="74" t="s">
         <v>347</v>
       </c>
-      <c r="B31" s="54" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="77" t="s">
+      <c r="B76" s="53" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="74" t="s">
         <v>348</v>
       </c>
-      <c r="B32" s="55" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="77" t="s">
+      <c r="B77" s="53" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="74" t="s">
         <v>349</v>
       </c>
-      <c r="B33" s="53" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="77" t="s">
+      <c r="B78" s="53" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="74" t="s">
         <v>350</v>
       </c>
-      <c r="B34" s="53" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="77" t="s">
+      <c r="B79" s="53" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="74" t="s">
         <v>351</v>
       </c>
-      <c r="B35" s="53" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="77" t="s">
+      <c r="B80" s="53" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="74" t="s">
         <v>352</v>
       </c>
-      <c r="B36" s="53" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="77" t="s">
+      <c r="B81" s="53" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="74" t="s">
         <v>353</v>
       </c>
-      <c r="B37" s="53" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="77" t="s">
+      <c r="B82" s="53" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="74" t="s">
         <v>354</v>
       </c>
-      <c r="B38" s="53" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="77" t="s">
+      <c r="B83" s="53" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="1:3" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A97" s="70">
+        <v>5</v>
+      </c>
+      <c r="B97" s="73" t="s">
         <v>355</v>
       </c>
-      <c r="B39" s="53" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="53"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="77" t="s">
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="74" t="s">
         <v>356</v>
       </c>
-      <c r="B50" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="77" t="s">
+      <c r="B98" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="74" t="s">
         <v>357</v>
       </c>
-      <c r="B53" t="s">
-        <v>284</v>
-      </c>
-      <c r="C53" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="77" t="s">
+      <c r="B99" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="74" t="s">
         <v>358</v>
       </c>
-      <c r="B57" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="77" t="s">
+      <c r="B100" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="74" t="s">
         <v>359</v>
       </c>
-      <c r="B59" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="77" t="s">
+      <c r="B101" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="74" t="s">
         <v>360</v>
       </c>
-      <c r="B65" s="53" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="77" t="s">
+      <c r="B102" t="s">
+        <v>291</v>
+      </c>
+      <c r="C102" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="74" t="s">
         <v>361</v>
       </c>
-      <c r="B66" s="53" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="77" t="s">
+      <c r="B103" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="74" t="s">
         <v>362</v>
       </c>
-      <c r="B67" s="53" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="53"/>
-    </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="53"/>
-    </row>
-    <row r="70" spans="1:2" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A70" s="70">
-        <v>4</v>
-      </c>
-      <c r="B70" s="73" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="77" t="s">
-        <v>364</v>
-      </c>
-      <c r="B71" s="53" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="77" t="s">
-        <v>365</v>
-      </c>
-      <c r="B72" s="53" t="s">
+      <c r="B104" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="77" t="s">
-        <v>366</v>
-      </c>
-      <c r="B73" s="53" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="77" t="s">
-        <v>367</v>
-      </c>
-      <c r="B74" s="53" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="77" t="s">
-        <v>368</v>
-      </c>
-      <c r="B75" s="53" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="77" t="s">
-        <v>369</v>
-      </c>
-      <c r="B76" s="53" t="s">
+      <c r="C104" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="77" t="s">
-        <v>370</v>
-      </c>
-      <c r="B77" s="53" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="77" t="s">
-        <v>371</v>
-      </c>
-      <c r="B78" s="53" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="77" t="s">
-        <v>372</v>
-      </c>
-      <c r="B79" s="53" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="93" spans="1:2" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A93" s="70">
-        <v>5</v>
-      </c>
-      <c r="B93" s="73" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="77" t="s">
-        <v>374</v>
-      </c>
-      <c r="B94" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="77" t="s">
-        <v>375</v>
-      </c>
-      <c r="B95" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="77" t="s">
-        <v>376</v>
-      </c>
-      <c r="B96" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="77" t="s">
-        <v>377</v>
-      </c>
-      <c r="B97" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="77" t="s">
-        <v>378</v>
-      </c>
-      <c r="B98" t="s">
-        <v>302</v>
-      </c>
-      <c r="C98" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="77" t="s">
-        <v>379</v>
-      </c>
-      <c r="B99" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="77" t="s">
-        <v>380</v>
-      </c>
-      <c r="B100" t="s">
-        <v>302</v>
-      </c>
-      <c r="C100" t="s">
-        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -13506,7 +13579,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="11"/>
@@ -13519,10 +13592,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -13534,10 +13607,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -13549,10 +13622,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -13563,7 +13636,7 @@
       <c r="A10" s="6"/>
       <c r="B10" s="11"/>
       <c r="C10" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -13575,7 +13648,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -13588,7 +13661,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="11"/>
@@ -13596,15 +13669,15 @@
       <c r="F12" s="13"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7" ht="258.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="258.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>7</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -13616,10 +13689,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
@@ -13631,10 +13704,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
@@ -13674,7 +13747,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="35.1" x14ac:dyDescent="0.45">
       <c r="B1" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="33" x14ac:dyDescent="0.45">
@@ -13702,7 +13775,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="11"/>
@@ -13715,10 +13788,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -13730,10 +13803,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="237" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -13741,10 +13814,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -13752,7 +13825,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="11"/>
@@ -13765,15 +13838,15 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13781,10 +13854,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -13792,7 +13865,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="11"/>
@@ -13805,7 +13878,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13813,10 +13886,10 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -13824,10 +13897,10 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="117" customHeight="1" x14ac:dyDescent="0.25">
@@ -13835,10 +13908,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -13864,7 +13937,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="35.1" x14ac:dyDescent="0.45">
       <c r="B1" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="33" x14ac:dyDescent="0.45">
@@ -13892,7 +13965,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="11"/>
@@ -13905,10 +13978,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -13920,10 +13993,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="186" customHeight="1" x14ac:dyDescent="0.2">
@@ -13931,10 +14004,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -13942,10 +14015,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -13953,7 +14026,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -13961,7 +14034,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.25">
@@ -13969,10 +14042,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add info to be able to see upload icon in admin console
</commit_message>
<xml_diff>
--- a/test/testcase/NORMAN Sanity Check.xlsx
+++ b/test/testcase/NORMAN Sanity Check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1020" windowWidth="25440" windowHeight="15990" activeTab="5"/>
+    <workbookView xWindow="840" yWindow="1020" windowWidth="25440" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisite" sheetId="6" r:id="rId1"/>
@@ -2522,6 +2522,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2531,10 +2535,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Bad" xfId="66" builtinId="27"/>
@@ -7593,8 +7593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7765,7 +7765,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="39">
         <v>3.1</v>
       </c>
@@ -7773,37 +7773,37 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="39">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="52"/>
+      <c r="B25" s="75" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="39">
         <v>3.2</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B26" s="41" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="39">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="39">
         <v>3.3</v>
       </c>
-      <c r="B26" s="41" t="s">
+      <c r="B27" s="41" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="52">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="52">
         <v>3.4</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="B28" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="78" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -9564,13 +9564,13 @@
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="79"/>
     </row>
     <row r="11" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
@@ -13025,8 +13025,8 @@
   </sheetPr>
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13056,7 +13056,7 @@
     </row>
     <row r="5" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="76" t="s">
         <v>389</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update file SAPUI name
</commit_message>
<xml_diff>
--- a/test/testcase/NORMAN Sanity Check.xlsx
+++ b/test/testcase/NORMAN Sanity Check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1020" windowWidth="25440" windowHeight="15990"/>
+    <workbookView xWindow="840" yWindow="1020" windowWidth="25440" windowHeight="15990" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisite" sheetId="6" r:id="rId1"/>
@@ -1180,9 +1180,6 @@
   </si>
   <si>
     <t>check 3 pages appear: Blank Page, ObjectPage, ListReport</t>
-  </si>
-  <si>
-    <t>Set version 1.31.0</t>
   </si>
   <si>
     <r>
@@ -1919,6 +1916,15 @@
     <t>3,22</t>
   </si>
   <si>
+    <t>to be able to see the UICatalogs icon on the admin console. update  Admin/server/config/features.json  put "Enabled:"TRUE</t>
+  </si>
+  <si>
+    <t>to be able to see the UICatalogs icon on the admin console. update  Admin/server/config/features.json  put "Enabled:"TRUE(: STEP explain in prerequisite sheet)</t>
+  </si>
+  <si>
+    <t>Set version 1.30.1</t>
+  </si>
+  <si>
     <r>
       <t>select</t>
     </r>
@@ -1931,7 +1937,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> devVersion.zip </t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dev2.zip</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -1944,18 +1972,12 @@
       <t>and click on Open</t>
     </r>
   </si>
-  <si>
-    <t>to be able to see the UICatalogs icon on the admin console. update  Admin/server/config/features.json  put "Enabled:"TRUE</t>
-  </si>
-  <si>
-    <t>to be able to see the UICatalogs icon on the admin console. update  Admin/server/config/features.json  put "Enabled:"TRUE(: STEP explain in prerequisite sheet)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2136,6 +2158,14 @@
       <b/>
       <sz val="36"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -7593,7 +7623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
@@ -7681,7 +7711,7 @@
         <v>3.5</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -7776,7 +7806,7 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="52"/>
       <c r="B25" s="75" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -7818,19 +7848,19 @@
     <row r="32" spans="1:3" s="67" customFormat="1" ht="53.1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="A32" s="66"/>
       <c r="B32" s="67" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="67" customFormat="1" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A33" s="66"/>
       <c r="B33" s="67" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="67" customFormat="1" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A34" s="66"/>
       <c r="B34" s="67" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -7864,7 +7894,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="64" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="35.1" x14ac:dyDescent="0.45">
@@ -9529,7 +9559,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="64" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="24" customFormat="1" ht="35.1" x14ac:dyDescent="0.45">
@@ -11652,7 +11682,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="64" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="35.1" x14ac:dyDescent="0.45">
@@ -12585,12 +12615,12 @@
   <sheetData>
     <row r="1" spans="1:6" s="65" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="65" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="35.1" x14ac:dyDescent="0.45">
       <c r="B2" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="33" x14ac:dyDescent="0.45">
@@ -12633,7 +12663,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12641,7 +12671,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12649,7 +12679,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12657,27 +12687,27 @@
         <v>6</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="58" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="59" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="57"/>
       <c r="B14" s="60" t="s">
+        <v>300</v>
+      </c>
+      <c r="C14" s="60" t="s">
         <v>301</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="D14" s="60" t="s">
         <v>302</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="E14" s="60" t="s">
         <v>303</v>
-      </c>
-      <c r="E14" s="60" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="383.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12687,45 +12717,45 @@
     </row>
     <row r="16" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="60" t="s">
+        <v>304</v>
+      </c>
+      <c r="C16" t="s">
         <v>305</v>
-      </c>
-      <c r="C16" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="383.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C17" s="60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="58" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="61"/>
       <c r="B19" s="62" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="57"/>
       <c r="B20" s="57" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="57"/>
       <c r="B21" s="60" t="s">
+        <v>309</v>
+      </c>
+      <c r="C21" s="60" t="s">
         <v>310</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="D21" s="60" t="s">
         <v>311</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="E21" s="60" t="s">
         <v>312</v>
-      </c>
-      <c r="E21" s="60" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="269.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12737,13 +12767,13 @@
     <row r="23" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="57"/>
       <c r="B23" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="C23" s="63" t="s">
         <v>314</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="D23" s="60" t="s">
         <v>315</v>
-      </c>
-      <c r="D23" s="60" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -13025,8 +13055,8 @@
   </sheetPr>
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13036,7 +13066,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="65" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="65" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.95" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -13057,7 +13087,7 @@
     <row r="5" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="76" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -13078,13 +13108,13 @@
     <row r="9" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="11" t="s">
-        <v>272</v>
+        <v>388</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13096,7 +13126,7 @@
     <row r="12" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="11" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13141,7 +13171,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -13149,10 +13179,10 @@
         <v>2.4</v>
       </c>
       <c r="B20" s="68" t="s">
+        <v>273</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>274</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13160,7 +13190,7 @@
         <v>2.5</v>
       </c>
       <c r="B21" s="68" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -13201,135 +13231,135 @@
         <v>3</v>
       </c>
       <c r="B28" s="73" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="74" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B29" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="74" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B30" s="53" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="74" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B31" s="53" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="74" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B32" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="74" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B33" s="54" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B34" s="55" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="74" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B35" s="53" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="74" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B36" s="53" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="74" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="74" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B38" s="53" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="74" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B39" s="53" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="74" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B40" s="53" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="74" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B41" s="53" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="74" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B42" s="53" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="74" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="74" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B44" s="53" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -13337,58 +13367,58 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="74" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B55" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="74" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B58" t="s">
+        <v>278</v>
+      </c>
+      <c r="C58" t="s">
         <v>279</v>
-      </c>
-      <c r="C58" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="74" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B62" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="74" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B64" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B70" s="53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="74" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B71" s="53" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="74" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B72" s="53" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
@@ -13402,79 +13432,79 @@
         <v>4</v>
       </c>
       <c r="B75" s="73" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="74" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B76" s="53" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="74" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B77" s="53" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="74" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B78" s="53" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="74" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B79" s="53" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="74" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B80" s="53" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="74" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B81" s="53" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="74" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B82" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="74" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B83" s="53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="74" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B84" s="53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -13483,69 +13513,69 @@
         <v>5</v>
       </c>
       <c r="B98" s="73" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="74" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B99" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="74" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B100" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="74" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B101" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="74" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B102" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="74" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B103" t="s">
+        <v>290</v>
+      </c>
+      <c r="C103" t="s">
         <v>291</v>
-      </c>
-      <c r="C103" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="74" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B104" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="74" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B105" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C105" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove sapui and update sanity check
</commit_message>
<xml_diff>
--- a/test/testcase/NORMAN Sanity Check.xlsx
+++ b/test/testcase/NORMAN Sanity Check.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="391">
   <si>
     <t>New Project</t>
   </si>
@@ -1916,9 +1916,6 @@
     <t>to be able to see the UICatalogs icon on the admin console. update  Admin/server/config/features.json  put "Enabled:"TRUE(: STEP explain in prerequisite sheet)</t>
   </si>
   <si>
-    <t>Set version 1.30.1</t>
-  </si>
-  <si>
     <t>init database: node server/initschema.js</t>
   </si>
   <si>
@@ -1961,12 +1958,18 @@
       <t>and click on Open</t>
     </r>
   </si>
+  <si>
+    <t>Set version 1.30.2</t>
+  </si>
+  <si>
+    <t>you can find the zip file https://jam4.sapjam.com/groups/60qDosrRAVDTLeeirVt451/content?folder_id=6pmalrbCS0ylIID3KNQGbW</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2154,6 +2157,14 @@
     <font>
       <i/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2405,7 +2416,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2545,6 +2556,8 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6308,13 +6321,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1876425</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>314325</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3067050</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6363,13 +6376,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>321412</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6418,13 +6431,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1943100</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3248025</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6473,13 +6486,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1657350</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6528,13 +6541,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6583,13 +6596,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1857375</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3019425</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6638,13 +6651,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1847850</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6693,13 +6706,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3714750</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>292610</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6150485</xdr:colOff>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7692,7 +7705,7 @@
         <v>3.4</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7700,7 +7713,7 @@
         <v>3.5</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -9587,13 +9600,13 @@
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="79"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="81"/>
     </row>
     <row r="11" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15">
@@ -13046,24 +13059,24 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.28515625" customWidth="1"/>
+    <col min="2" max="2" width="147.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="65" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:3" s="65" customFormat="1" ht="51.95" x14ac:dyDescent="0.65">
       <c r="B1" s="65" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.95" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" s="72" customFormat="1" ht="26.1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="15.95" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" s="72" customFormat="1" ht="26.1" x14ac:dyDescent="0.35">
       <c r="A3" s="70">
         <v>1</v>
       </c>
@@ -13071,503 +13084,520 @@
         <v>212</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="11" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="76" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="11" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="11" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="11" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="11" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="11" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="11" t="s">
+    </row>
+    <row r="14" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="6"/>
+      <c r="B15" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="C15" s="77"/>
+    </row>
+    <row r="16" spans="1:3" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="78" t="s">
+        <v>390</v>
+      </c>
+      <c r="C16" s="77"/>
+    </row>
+    <row r="17" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="11" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="13" customFormat="1" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13" t="s">
+    <row r="18" spans="1:3" s="13" customFormat="1" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.95" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:2" s="72" customFormat="1" ht="26.1" x14ac:dyDescent="0.35">
-      <c r="A16" s="70">
+    <row r="19" spans="1:3" ht="15.95" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:3" s="72" customFormat="1" ht="26.1" x14ac:dyDescent="0.35">
+      <c r="A20" s="70">
         <v>2</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B20" s="73" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>2.1</v>
-      </c>
-      <c r="B17" s="68" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B18" s="68" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B19" s="68" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="B20" s="68" t="s">
-        <v>272</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="B21" s="68" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B22" s="68" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B23" s="68" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="B24" s="68" t="s">
+        <v>272</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
         <v>2.5</v>
       </c>
-      <c r="B21" s="68" t="s">
+      <c r="B25" s="68" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="68"/>
-    </row>
-    <row r="23" spans="1:3" s="13" customFormat="1" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="69"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="53"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="53"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="68"/>
+    </row>
+    <row r="27" spans="1:3" s="13" customFormat="1" ht="15.95" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="69"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="53"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="53"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>2.6</v>
       </c>
-      <c r="B26" s="53" t="s">
+      <c r="B30" s="53" t="s">
         <v>268</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C30" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>2.7</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B31" s="53" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A28" s="70">
+    <row r="32" spans="1:3" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A32" s="70">
         <v>3</v>
       </c>
-      <c r="B28" s="73" t="s">
+      <c r="B32" s="73" t="s">
         <v>322</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="74" t="s">
-        <v>323</v>
-      </c>
-      <c r="B29" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="74" t="s">
-        <v>324</v>
-      </c>
-      <c r="B30" s="53" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="s">
-        <v>325</v>
-      </c>
-      <c r="B31" s="53" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="74" t="s">
-        <v>326</v>
-      </c>
-      <c r="B32" s="54" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="74" t="s">
-        <v>327</v>
-      </c>
-      <c r="B33" s="54" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="56" customFormat="1" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+      <c r="B33" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="74" t="s">
-        <v>328</v>
-      </c>
-      <c r="B34" s="55" t="s">
-        <v>363</v>
+        <v>324</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="74" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B35" s="53" t="s">
-        <v>365</v>
+        <v>275</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="74" t="s">
-        <v>330</v>
-      </c>
-      <c r="B36" s="53" t="s">
-        <v>364</v>
+        <v>326</v>
+      </c>
+      <c r="B36" s="54" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="74" t="s">
-        <v>331</v>
-      </c>
-      <c r="B37" s="53" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+      <c r="B37" s="54" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="74" t="s">
-        <v>332</v>
-      </c>
-      <c r="B38" s="53" t="s">
-        <v>366</v>
+        <v>328</v>
+      </c>
+      <c r="B38" s="55" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="74" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B39" s="53" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="74" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B40" s="53" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="74" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B41" s="53" t="s">
-        <v>369</v>
+        <v>321</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="74" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B42" s="53" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="74" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="74" t="s">
+        <v>334</v>
+      </c>
+      <c r="B44" s="53" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="74" t="s">
+        <v>335</v>
+      </c>
+      <c r="B45" s="53" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="74" t="s">
+        <v>336</v>
+      </c>
+      <c r="B46" s="53" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="74" t="s">
+        <v>337</v>
+      </c>
+      <c r="B47" s="53" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="74" t="s">
         <v>338</v>
       </c>
-      <c r="B44" s="53" t="s">
+      <c r="B48" s="53" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="53"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="74" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="53"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="74" t="s">
         <v>339</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B59" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="74" t="s">
-        <v>340</v>
-      </c>
-      <c r="B58" t="s">
-        <v>277</v>
-      </c>
-      <c r="C58" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="74" t="s">
+        <v>340</v>
+      </c>
+      <c r="B62" t="s">
+        <v>277</v>
+      </c>
+      <c r="C62" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="74" t="s">
         <v>341</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B66" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="74" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="74" t="s">
         <v>381</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B68" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="53" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="53" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="74" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="74" t="s">
         <v>382</v>
       </c>
-      <c r="B71" s="53" t="s">
+      <c r="B75" s="53" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="74" t="s">
+    <row r="76" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="74" t="s">
         <v>383</v>
       </c>
-      <c r="B72" s="53" t="s">
+      <c r="B76" s="53" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="53"/>
-    </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="53"/>
-    </row>
-    <row r="75" spans="1:2" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A75" s="70">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="53"/>
+    </row>
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="53"/>
+    </row>
+    <row r="79" spans="1:2" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A79" s="70">
         <v>4</v>
       </c>
-      <c r="B75" s="73" t="s">
+      <c r="B79" s="73" t="s">
         <v>342</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="74" t="s">
-        <v>343</v>
-      </c>
-      <c r="B76" s="53" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="74" t="s">
-        <v>344</v>
-      </c>
-      <c r="B77" s="53" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="74" t="s">
-        <v>345</v>
-      </c>
-      <c r="B78" s="53" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="74" t="s">
-        <v>346</v>
-      </c>
-      <c r="B79" s="53" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="74" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B80" s="53" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="74" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B81" s="53" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="74" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B82" s="53" t="s">
-        <v>282</v>
+        <v>377</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="74" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B83" s="53" t="s">
-        <v>283</v>
+        <v>378</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="74" t="s">
+        <v>347</v>
+      </c>
+      <c r="B84" s="53" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="74" t="s">
+        <v>348</v>
+      </c>
+      <c r="B85" s="53" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="74" t="s">
+        <v>349</v>
+      </c>
+      <c r="B86" s="53" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B87" s="53" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="74" t="s">
         <v>351</v>
       </c>
-      <c r="B84" s="53" t="s">
+      <c r="B88" s="53" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="1:3" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A98" s="70">
+    <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:3" s="72" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A102" s="70">
         <v>5</v>
       </c>
-      <c r="B98" s="73" t="s">
+      <c r="B102" s="73" t="s">
         <v>352</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="74" t="s">
-        <v>353</v>
-      </c>
-      <c r="B99" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="74" t="s">
-        <v>354</v>
-      </c>
-      <c r="B100" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="74" t="s">
-        <v>355</v>
-      </c>
-      <c r="B101" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="74" t="s">
-        <v>356</v>
-      </c>
-      <c r="B102" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="74" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B103" t="s">
-        <v>289</v>
-      </c>
-      <c r="C103" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="74" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B104" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="74" t="s">
+        <v>355</v>
+      </c>
+      <c r="B105" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="74" t="s">
+        <v>356</v>
+      </c>
+      <c r="B106" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="74" t="s">
+        <v>357</v>
+      </c>
+      <c r="B107" t="s">
+        <v>289</v>
+      </c>
+      <c r="C107" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="74" t="s">
+        <v>358</v>
+      </c>
+      <c r="B108" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="74" t="s">
         <v>359</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B109" t="s">
         <v>289</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C109" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>